<commit_message>
Upload images and csv files
</commit_message>
<xml_diff>
--- a/training_data.xlsx
+++ b/training_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Deep Learning or WTF\MultiModal-Classifying\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0064FE28-42C5-43E9-8A3F-BBA22C7F5CC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A4CFA8-29D0-428F-BAC7-98A58B2A4030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{40A742FA-D448-404E-963F-390F22E97DD1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{40A742FA-D448-404E-963F-390F22E97DD1}"/>
   </bookViews>
   <sheets>
     <sheet name="training_data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="604">
   <si>
     <t>img_path</t>
   </si>
@@ -2162,6 +2162,971 @@
   <si>
     <t>imgamazon\612MpjJOHFL._AC_SX679_.jpg</t>
   </si>
+  <si>
+    <t>imgamazon\613G3YAzwgL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>24H HEALTH FOLLOW UP: Automated heart rate measurement, 24-hour heart rate monitor, resting heart rate, exercise heart rate, heart rate alert, stress monitor, sleep monitor, steps throughout the whole day, calories, distance, exercise duration
+SEAMLESS FROM WATCH TO APP: Unlock the whole CMF experience with the CMF Watch app. From managing your device to checking your fitness and health stats, it's a seamless extension to your watch
+BUILT-IN MULTI-SYSTEM GPS: Go places, with built-in GPS. With support for 5 satellite positioning systems, you can effortlessly obtain accurate trace and distance data for activities such as running, cycling, walking and hiking.
+BIG SCREEN POTENTIAL: More than just timekeeping. Carry everything from fitness tracking to smart notifications on your wrist with the CMF Watch Pro. The expansive 1.96" AMOLED display magnifies your information through ultra smooth touch-responsive interactions. All it takes is a tap.
+MORE FUNCTION:Bluetooth call, Cloud watch dials, photo album dials, breathing training, message notification, phone music control, timer, stopwatch, alarms, weather, find my phone, flashlight, remote camera control Microphone: Supported, Speaker: Supported, Water &amp; Dust Resistance Rating: IP68</t>
+  </si>
+  <si>
+    <t>imgamazon\71tDuqXXYOL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>All-Round Health Monitor,Your Health Journey: CMF Smart Watch Pro 2 is a portable blood oxygen saturation monitor designed for both men and women. The heart monitor tracks your heart rate continuously for 24 hours a day, along with recording sleep patterns, stress levels, and SpO₂ levels. Seamlessly sync and manage your fitness data across Apple Health, Google Health Connect, and Strava. You can also synchronize data between your app and the watch for comprehensive health tracking.
+Bluetooth Calls and Gesture Control:The CMF Smartwatch enables crystal-clear Bluetooth phone calls with enhanced AI noise reduction technology. Equipped with a built-in microphone and speaker, the Watch Pro 2 ensures seamless communication. You can add and manage up to 30 contacts on your watch, allowing you to handle calls directly from your wrist. Real-time message reminders are also supported.The new gesture control feature allows one-handed operation of the watch using wrist movements. For example, flipping your wrist once or twice can trigger customized functions such as answering/rejecting/ignoring incoming calls, skipping to the next/previous music track, performing other operations.
+Interactive Design with Interchangeable Bezels and Straps:The CMF Watch Pro 2 features a 1.32" AMOLED display that delivers sharp, vibrant visuals with enhanced resolution (466 x 466), 353 PPI, and a refresh rate of 60Hz. It is a stylish and feature-packed smartwatch offering an interchangeable bezel design and removable watch straps, allowing effortless switching between styles to suit any occasion. With over 100 signature watch faces and customizable options, you can create personalized combinations.
+120 Sports Modes with IP68 Waterproof: The CMF fitness tracker smartwatch is IP68 waterproof and supports 120 sports modes, including smart automatic recognition of 5 common activities. It features a 3D warm-up exercise guide and 'My Heart Rate' for personalized heart rate zones. The Smart Movement Algorithm tracks sports data, measures aerobic and anaerobic training effectiveness, training load, and recovery time. Fitness data can be seamlessly shared with Apple Health, Google Health Connect, and Strava.
+Smoothly Watch APP and More Performance: Enjoy seamless connectivity with the CMF Watch app. Manage and control your preferred features with a long battery life of up to 11 days. The watch offers smart functionalities including notifications, quick Android SMS replies, find my phone, camera control, alarms, timers, weather forecasts, music control, and multi-system GPS.
+For accurate GPS positioning, ensure you're in an open area, connect to the app at least every 7 days, avoid locations with potential signal interference or large public transportation systems, and maintain a proper connection between your watch and phone.</t>
+  </si>
+  <si>
+    <t>imgamazon\51OFELc9svL._AC_.jpg</t>
+  </si>
+  <si>
+    <t>1.47" HD Color Screen and 100+ DIY Dial: Smart watch is equipped with a 172*320 extra-large hd full touch color screen, delivering exceptional picture quality and highly responsive touch sensitivity, which can bring you a unique visual and better interactive experience, with the companion “Gloryfit” app, you can download more than 100 free personalised watch faces and set it as your desktop for fitness tracker.
+Message Notifications: Smartwatches is equipped with built-in hd speaker, after connecting to your smartphone via bluetooth, you can view call history. The smart watch for men also provides notifications of social media messages including facebook, whatsApp, instagram, twitter, etc. Through vibrating alerts. So that you will never miss any important information.
+24-Hour Health Monitoring: Smartwatch adopting advanced sensors, accurately monitors your heart rate in real time and Spo2, and it will monitor your sleep status automatically period around and provides comprehensive sleep quality analysis. Synchronize to the mobile phone app"Gloryfit", you can understand your sleep status(deep /light /wakeful sleep) by Smart watches develop a better sleep habit and a healthier lifestyle.
+24+ Sports Modes and IP68 Waterproof: Fitness watch supports multiple sports modes, including running, cycling, walking, basketball, yoga, football and so on. During your exercise, activity tracker will record your data like, steps, calories burned, etc. Sport watch is ip68 waterproof rating, ensuring worry-free use even while washing hands, face, or engaging in sweaty activities. However, it is not recommended for use in hot water or seawater.
+Multifunctional and Long Battery Life: smart watch for women for men has multiple functions such as timer, stopwatch, alarm clock, find your phone, sedentary reminder, music control, weather forecast, don‘t disturb mode, brightness adjustment, female cycle tracking. The sport tracker with 3 hrs of charging, 3-5 days of normal use and about 30 days of standby time. The fitness tracker compatible with ios 9.0 and android 6.0 and above devices.</t>
+  </si>
+  <si>
+    <t>imgamazon\717a9oQOajL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>Bluetooth Calling and Message Viewing: This smart watch features bluetooth version 5.3 for faster connectivity. You can make/receive calls with the built-in microphone and speaker. You can also receive and view message notifications through the watch.
+1.85” HD Display and DIY Watch Face: The smart watches for men has 1.85 inch high definition screen allows you to have a different visual enjoyment. This smart watches has the ability to customize the watch face. You can create one what you like.
+24/7 All-round Health Monitoring: This fitness tracker has 24/7 all-around health monitoring, tracking your health data in real time through precise sensors. You can always know your physical condition and adjust your lifestyle habits based on the data.
+120+ Sports Modes: Sports watch supports more than 120+ sports modes, including running, walking, hiking, badminton, basketball, rowing, hiking, cycling, fitness, football. Swimming, yoga, etc.
+IP68 Waterproof: The with an IP68 waterproof rating, this smartwatch ensures worry free use even when washing your hands, face or sweating (note: not suitable for prolonged immersion in water).
+Battery Life: The smart watchs has a built in 350 mAh rechargeable battery that can be fully charged in just 2 hours and lasts up to 8-10 days (Depends on actual use), up to 20 days in power saving mode and up to 30 days in standby mode.
+Broad compatibility: The fitness watch is compatible with all major systems such as Android 4.4 and iOS 9.0 or later smartphones (not suitable for PCs or tablets).</t>
+  </si>
+  <si>
+    <t>imgamazon\71mpuO4LqeL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>Stylish Design, Bright Display: The sleek stainless steel build blends classic style with workout durability, while the bright 1.32" AMOLED display keeps your data easy to read, even under bright sunlight.
+Precise Heart Rate &amp; Sleep Tracking: Amazfit's BioTracker technology tracks your heart rate and sleep data with accuracy that previous sensors just can't match.
+Up to 10 Days of Battery Life: With long battery life that lasts up to 10 days with typical use, nightly recharges are a thing of the past.
+Free Maps with Turn Directions: Stay on-track with free downloadable maps, and get turn-by-turn guidance on-screen or via your Bluetooth headphones. Enjoy ski maps for global resorts, including guidance for cable cars, slopes, and more.
+Faster and More Accurate GPS Tracking: 5 satellite positioning systems ensure fast GPS connection and accurate positioning whenever you're out running, walking, cycling or hiking.
+Over 160 Sports Modes: The Amazfit Active 2 smart watch offers 160+ workout modes, including HYROX Race, Strength Training, running, padel, and yoga. With 50m water-resistance and a barometer, go swimming and skiing with confidence.
+Free and Safe Zepp App: Featuring no hidden mandatory subscription fees, the Zepp App benefits from industry-leading data protection by AWS with GDPR compliance. Find all your health and fitness data, along with actionable insights, in one place.
+Speech-to-Text Message Replies: Zepp Flow offers full voice control of your smartwatch. Use it to send replies to Android messages using speech-to-text or keyboard input - it can even help with translations and tone suggestions.
+Choose Your Look: The Premium version features resilient sapphire glass, a luxurious leather strap, and a free additional silicone sport band. The Sport version features a breathable silicone strap in black or red, for comfort during workouts.</t>
+  </si>
+  <si>
+    <t>imgamazon\71paa6esk2L._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>1.96" HD Big Screen and Unlimited Customization Dials: smart watches for women adopt 1.96”TFT HD color display screen (320*386 resolution) which making it easy to operate and sensitive, experience crystal-clear visuals like never before. 4 level brightness adjustable allows you to read time and data clearly even under the glare. 200+ Multiple trendsetting combinations to match your mood and outfit of the day. Even create and customize your own mens smart watch faces from your phone gallery.
+2025 New Smart Watch with Bluetooth Call/Intelligent Notifications: The smart watches for men adopts bluetooth 5.3 version for a faster and more stable connection. With a built-in premium microphone and hd speaker, allowing you to answer calls and interact with voice assistants directly from smartwatch. Meanwhile, you can receive message notifications and read them from your watch, such as Facebook, Messenger, Instagram, Gmail, Whatsapp, Twitter etc. Just raise your wrist to view messages.
+24/7 Heart Rate Monitor and Sleep Tracker: Adopted high-performance optical sensors, Fitness tracker provides health monitoring features such as 24-hour continuity real-time Heart Rate, SpO2, and Sleep Monitoring(Deep/light sleep). It accurately monitors your heart rate in real time nd better understand your heart rate trends. Also, it provides a detailed analysis of your sleep quality and facilitating lifestyle adjustments by "GloryFit" continuously recording your sleep patterns.
+110+ Multiple Fitness Modes and IP68 Waterproof: The waterproof watch supports 110+ sports modes indoors and outdoors (covering walking, cycling, hiking, yoga, etc). At the sametime, Connecting the GPS in your cellphone can track all your workout routes and physical status during exercise. The smartwtach men is IP68 waterproof, you can wear it when washing hands, in the rain(Note: Do Not use in showers, saunas, etc).
+30-day Standby Time and Wide Compatibility: The well-designed and detachable wristband which soft, lightweight, breathable and very comfortable when wearing. Beside, the android smart watch is designed with a large-capacity battery, Charging time is 1.5-2 hours，once charge which allows it to last about 5-7 days for daily use and 30 days on standby mode. P99 smart watches compatible with most android and iOS phone (andriod 6.0+ and iOS 10.0+).</t>
+  </si>
+  <si>
+    <t>imgamazon\71rJzj8iaJL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>Back to Wrist Communication: Stay seamlessly connected to the Smart watch to make/answer Bluetooth calls and receive SMS and APP messages (Facebook, WhatsApp, Twitter, etc.) - convenient for your life and never miss important notifications again. Note: After connecting Bluetooth, please turn on message and call notification in GloryFit APP (you cannot send messages or texts back)
+24-Hour Health Activity Tracker: Prioritize your well-being with smart watches for men continuous health monitoring. Smart watches for women track your Heart Rate, Blood Oxygen levels(SpO2) and Sleep patterns (deep sleep, light sleep, REM analysis, get a better sleep habit by viewing your sleep data)around the clock. Take charge of your wellbeing and make informed decisions for a healthier lifestyle
+120+Sport Modes and 5ATM Waterproof: Achieve your fitness goals with over 120 sport modes (snowboarding, running, trail running, cycling, swimming, etc.) tailored to your workout. Smart watches for men record calories burned, number of steps, training time and distance for a variety of activities. Smart watches for women are also water-resistant up to 5 ATM, making it your ideal training partner
+Up to 10 days of battery life: Watches for women equipped with a powerful 300mAh battery, which enables a usage time of 7-10 days after just 2.5 hours of charging. This provides reliable support for everyday use and outdoor activities. Watches for men it is compatible with Android 6.0 and higher and iOS 10.0 and higher (only for phones, not for PCs, iPads or tablets)
+Voice and life assistant: Enjoy the convenience of the voice assistant, your virtual assistant right on your wrist. Ask questions, set reminders, control smart devices and much more, all with your fitness tracker.There are also some life functions such as: Flashlight, alarm clock, stopwatch, camera and music control, lack of exercise reminder, breathing training, women's health, phone search, mini games and much more
+1.83 Color screen &amp; 500+ watch face: Womens watch with 1.83-inch touch screen and 4-level adjustable brightness, clearer display in sunlight, more convenient operation. Mens watches have more than 500+ unique online watch faces to choose from, you can also choose any picture on your phone as wallpaper to show your personal style
+More for every customer: Inside the package 3 replacement wristbands: one nylon replacement wristbands, one sport replacement wristbands, one silicone replacement wristbands, meet your different needs. If you have any problems, please contact us via Amazon, professional customer service will help you solve it Within 24 hours.</t>
+  </si>
+  <si>
+    <t>imgamazon\71Z1LMj3QmL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>2025 New Smart Watch with Bluetooth Call/Intelligent Notifications: The smart watches for men adopts bluetooth 5.3 version for a faster and more stable connection. With a built-in premium microphone and hd speaker, allowing you to answer calls and interact with voice assistants directly from smartwatch. Meanwhile, you can receive message notifications and read them from your watch, such as Facebook, Messenger, Instagram, Gmail, Whatsapp, Twitter etc. Just raise your wrist to view messages.
+1.96" HD Big Screen and Unlimited Customization Dials: smart watches for women adopt 1.96”TFT HD color display screen (320*386 resolution) which making it easy to operate and sensitive, experience crystal-clear visuals like never before. 4 level brightness adjustable allows you to read time and data clearly even under the glare. 200+ Multiple trendsetting combinations to match your mood and outfit of the day. Even create and customize your own mens smart watch faces from your phone gallery.
+24/7 Heart Rate Monitor and Sleep Tracker: Adopted high-performance optical sensors, Fitness tracker provides health monitoring features such as 24-hour continuity real-time Heart Rate, SpO2, and Sleep Monitoring(Deep/light sleep). It accurately monitors your heart rate in real time nd better understand your heart rate trends. Also, it provides a detailed analysis of your sleep quality and facilitating lifestyle adjustments by "GloryFit" continuously recording your sleep patterns.
+All Day Activity and Practical Functions: During exercise, sport smart watch automatically records daily steps, distance counter，calories burned, active minutes. This fitness watch men has other useful features offered like remote camera, music control, weather forecast, sedentary reminder, GPS tracking, stopwatch, find phone, raise to wake, alarm clock, calculator, etc. It makes things on your wrist simple and easy, and will always work as your effective daily assissant.
+110+ Multiple Fitness Modes and IP68 Waterproof: The waterproof watch supports 110+ sports modes indoors and outdoors (covering walking, cycling, hiking, yoga, swimming, etc). At the sametime, Connecting the GPS in your cellphone can track all your workout routes and physical status during exercise. The smartwtach men is IP68 waterproof, you can wear it when washing hands, in the rain(Note: Do Not use in showers, saunas, etc).
+30-day Standby Time and Wide Compatibility: The well-designed and detachable wristband which soft, lightweight, breathable and very comfortable when wearing. Beside, the android smart watch is designed with a large-capacity battery, Charging time is 1.5-2 hours，once charge which allows it to last about 5-7 days for daily use and 30 days on standby mode. P99 smart watches compatible with most android and iOS phone (andriod 6.0+ and iOS 10.0+).</t>
+  </si>
+  <si>
+    <t>imgamazon\61I22cL7v+L._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>Personalized Watch Faces with Practical Tools: The fitness watch for women comes with theme dials and you can personalize the watch face to your liking and customize the display content. Brightness adjustment make you an optiomal experience based on environment change. The smartwatch features practical tools such as stopwatch, timer, music control, breathing training, night mode, alarm clock and wrist up awake, giving more convenience and fun to your life.
+Healthy Monitor on Your Wrist: The smartwatch monitors your heart rate in real time and you can view recorded data on the watch or App. Our watch also allows for manual detection of blood oxygen. Besides, the fitness watch tracks your sleep status automatically, including light sleep, deep sleep and awake time, helping you develop healthy sleep habits and improve sleep quality.
+Multiple Sport Modes with Waterproof: Our fitness watch is equipped with 10 different sports modes suan as yoga, walking, running, ect, tracking automatically your steps, distance, calorie burn, and activity time. The smartwatch also can track your outdoor workout route if connected with your smartphone's GPS. The sport watch features IP68 waterproof rating, ensuring that it can withstand sweat, hand washing, or rain in daily life, and is also suitable for swimming and diving.
+Get Notified on Smartwatches: The smart watch receives incoming call and notifications from SMS, Facebook, Instagram, Whatsapp etc, This helps you stay up-to-date and avoid missing important information. (The watch can not make calls or text back). The watch also has a sedentary reminder function and you can create reminders for drinking water, meetings, dinners, appointments and more in the alarm settings, enjoying a healthier lifestyle and a well-planned schedule.
+Long-lasting battery and Extensive Compatibility: The smart watch will take 2 hours to charge and last for up to 7 days of continuous use or 30 days standby time. The watch is compatible with smartphones that run on iOS 10.0 or Android OS 5.0 and have Bluetooth 4.0 or higher. Please note that it is not compatible with tablets or computers.
+Gentle Reminders for Users: Please do not wear the watch too tightly to avoid excessive friction may scratch the skin. Make your watch a rest after prolonged use.</t>
+  </si>
+  <si>
+    <t>imgamazon\61OEuoqFqYL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>Get inspired and stay accountable with Versa 4 + Premium - learn when to work out or recover, see real-time stats during exercise and find new ways to keep your routine fresh and fun.Operating temperature: -14° to 113°F. Radio transceiver: Bluetooth 5.0.Maximum operating altitude : 28,000 feet (8,534 m).
+Built for better fitness results: Daily Readiness Score(1), built-in GPS and workout intensity map, Active Zone Minutes, all-day activity tracking and 24/7 heart rate, 40+ exercise modes and automatic exercise tracking, water resistant to 50 meters
+Tools to measure and improve sleep quality: personalized Sleep Profile(1), daily sleep stages &amp; Sleep Score, smart wake alarm and do not disturb mode. Compatibility-Apple iOS 15 or higher, Android OS 9 or higher
+Maintain a healthy body and mind: daily Stress Management Score, reflection logging, SpO2(2), health metrics dashboard(3), guided breathing sessions, menstrual health tracking and mindfulness content
+Designed for fitness &amp; beyond: on-wrist Bluetooth calls, texts and phone notifications(4), customizable clock faces, Fitbit Pay(5), Amazon Alexa built-in(6), Google Wallet &amp; Maps (Google Maps Android only, coming Spring 2023 to iOS), 6+ day battery(7)
+Includes a 6-month Premium membership complete with personalized insights, advanced analytics, guided programs and more (New &amp; returning Premium users only. Must activate trial within 60-days of device activation. Content and features may change)</t>
+  </si>
+  <si>
+    <t>imgamazon\71pbEc1KO3L._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>Call Receiving/Dialing &amp; Read Message-Smart watch is equipped with a high-quality speaker, after connecting to Bluetooth, can directly use the watch to answer make calls/play music/read messages/store contacts/view call history. Smart watches for men /women allow you to exercise, fitness, and bike hands-free while never missing any calls &amp; messages during meetings or workouts. Android/iPhone smart watch can also receive other notifications, such as WhatsApp, Twitter, Facebook, Instagram, etc.
+All-day Health Monitoring-The activity tracker smart watch can detect your blood pressure/blood oxygen/heart rate/pressure&amp;breathing at rest in real-time. You can enable 24-hour heart rate detection in the APP. Smartwatch monitors sleep status (deep sleep, light sleep, and wake-up time) and provides comprehensive sleep quality analysis. It can also record and predict a girl's physiological period. With this fitness watch for men and women, you can have a healthier, more active life.
+100+ Sports Modes &amp; Multifunctional-Step tracker watch for men supports 100+ sports modes, which cover both common sports like running, and cycling, as well as more specialized sports. Keeps accurate records of steps, travel distance, and calories burned. Smart watch for Android phones have many daily practical functions like, weather information, music playback, camera control, alarm clock, stopwatch, breathing training, find phone, sedentary/drink reminder, calculators, AI control, and games.
+IP67 Waterproof &amp; Broad Compatibility--The waterproof smartwatch meets the IP67 waterproof standard. You can wear it while washing your hands, running in the rain, Not suitable for swimming, diving and bathing. (Do not let the watch soak in seawater and hot water, such as hot springs) It can support most Android and iOS phones(Android 5+, iOS 9+). It can be used for 5-7 days when fully charged, and the standby time is over 30 days with a 290 mAh large-capacity battery.
+1.9" Large Screen &amp; 100+ Dials--This fitness smart watch has a 1.83" HD full-rounded touch screen. Adjustable brightness allows you to easily read in the sun or the dark. We have carefully designed beautiful UI and more than 100 watch faces for you, allowing you to switch watch face styles through the App (Da fit) to design your style dial. It supports 28 languages. Please use a 5V charger to fully charge the watch before turning it on.</t>
+  </si>
+  <si>
+    <t>imgamazon\71FgFCzp-6L._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>Bluetooth Call and Message Reminder: The smart watch is equipped with microphone and Hi-Fi speaker, after connecting to FitCloudPro APP, you can directly use the watch to answer/make calls. The smart watch for men will notify you immediately, when your smartphone receives notifications of incoming calls, SMS, Whatsapp, Facebook, email and other app messages so that you will never miss any important information
+40mm HD colour Display and Customized Dials: smart watch has an ultra-thin 40mm AMOLED touch screen with ultra-high definition resolution of 466*466. which offers you a better visual and operation experience. The smart watch for women has 100+ free watch faces that can be downloaded and used in the app. In addition, you can select your favorite photo as a wallpaper.
+IP68 Waterproof and 100+ Sports Modes: The fitness tracker can provide 100+ exercise modes, such as running, yoga, outdoor sports, ball games, jumping jack, sit-ups, etc. It will record your data like heart rate, steps, calories burned, distance and active hours in real time. With an IP68 water resistance rating, this smartwatch can be worn even in the rain or when washing hands.
+24/7 Accurate Health Monitoring and Sleep Tracking: This fitness watch had advanced sensors which helps you detect heart rate ,SpO2 throughout the day, helping you understand your health status. In addition, it will also automatically monitor your sleep (deep sleep, light sleep, awakening), you can see the relevant data analysis on "FitCloudPro" and adjust your lifestyle to cultivate a healthy lifestyle.
+Long Battery Life and Multi-Functions: Womens/mens smart watch has a built-in 300 mhA large capacity battery, which can be fully charged in 2 hours, can be used for up to 7 days and has a long standby time of about 30 days. On the other hand, watch have many practical tools, such as weather forecasts, timer, find phone, women health, sedentary reminder, ect. Compatible with iOS 9.0 or above, Android 6.0 or above.</t>
+  </si>
+  <si>
+    <t>imgamazon\61d8niGcVrL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>See everything clearly with large, easy-to-read text on the bright AMOLED display that includes an always-on mode, perfect for quick glances
+With up to 11 days of battery life in smartwatch mode, you won’t have to take your watch off every night to charge — which means a more complete 24/7 picture of your health
+Health is important to you, so monitor everything from your Body Battery energy levels, sleep score, respiration, hydration and stress to women’s health, heart rate and more (This device is intended to give an estimate of your activity and metrics)
+Find new ways to keep your body moving with more than 25 built-in indoor and GPS sports apps, including walking, running, cycling, HIIT, swimming, golf and many more
+Never miss a call, text or social media alert from your paired Apple or Android smartphone with smart notifications delivered right to your wrist
+Use free preloaded workouts that include cardio, yoga, strength, HIIT and even Pilates; create your own in the Garmin Connect smartphone app, or try Garmin Coach free adaptive training plans to help you prepare for your next running challenge
+With a supported bank, leave your cash and cards at home; Garmin Pay contactless payments let you pay for purchases on the go
+Head out with peace of mind with safety and tracking features, including incident detection (during select activities) and Assistance, both of which send messages with your live location to emergency contacts (Requires setup and your smartphone to be in an area with network coverage where data connectivity is available)
+Personalize with watch faces, apps and widgets from our Connect IQ Store, and review your health and fitness data in detail with the free Garmin Connect smartphone app</t>
+  </si>
+  <si>
+    <t>imgamazon\817QHxxq34L._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>RUGGED. RELIABLE. READY FOR ANYTHING: Climb the highest peak; Bike the long way home; The durable titanium design is our toughest yet, able to stand up to the rigors of your workout, including rainy or dusty conditions — even ocean swimming¹
+USE YESTERDAY TO BEAT TODAY: Meet your biggest competition — you; Challenge yourself to perform at your peak on your next run or bike ride using tracking with Galaxy AI²; It lets you compare your current performance to your last one³
+KNOW YOUR SCORE. OWN YOUR DAY: Get personalized insights that help you perform at your peak every day; Know your physical readiness using Energy Score with Galaxy AI²; It calculates a score based on yesterday’s sleep, heart rate and steps⁴
+PERSONALIZED TIPS TO UNLOCK THE BEST YOU: Stay at your best using daily personalized suggestions from Wellness Tips⁵; Gain information based on insights collected by your Watch and analyzed on your phone
+MORE PRECISE HEART RATE TRACKING: Zero in on more precise readings during workouts using Heart Rate Tracking with Galaxy AI⁴ that filters out the physical movements of your body; Insights are collected by your Watch and analyzed on your phone</t>
+  </si>
+  <si>
+    <t>imgamazon\71NrPRCvFRL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>【IP68 Waterproof Multifunctinal Smart Watch】Torjalph fitness activity tracker smart watch is IP68 waterproof technology ,you can wear it when swimming,handwashing,it's rain-proof which means that you perform multiple exercise modes outside without worrying about sweat or rain corroding your fitness smart watch,and this watch equipped with a 230 mAh large capacity battery magnetic charging ,and this sports activity tracker watch can be used 5-7 days If fully charged.
+【Larger 1.83'' Full Screen Watch &amp; Multi-dial Selection】1.83 inch full HD color touch screen smart watch for men / women provides excellent 240*284 resolution image quality ,This Bluetooth smart watch offers a better touch experience and remarkable immersion and ,more than 200 watch faces for you to choose from App"Da Fit ", you can change the dial style according to your mood to wear keeping the world on your wrist
+【Accurate Activity Tracker Smart Watch 】sports watch activity tracker uses sweat and dust resistant breathable silicone strap, our Fitness Tracker Smart Watch for Android iOS Phones supports 12 sports modes,walking,running,bicycle,swimming,badminton,basketball,football,rope skipping. This bluetooth calls smart watch for men women is lightweight and stylish, bringing more convenient and relaxing sports experience while also providing more protection.
+【Your 24 Hour Personal Daily Health Monitor】Fitness watch for women men full touch screen IP67 waterproof bluetooth smartwatch for Android iOS Phones with heart rate blood pressure monitor multifunction Andriod smart watch with steps counter sleep monitor sports fitness watch, monitoring blood oxygen saturation allows you to understand your physical condition in real time to track fitness progress ,to know your health status in time.
+【More Functions Bluetooth Call Smart Watch】This fitness activity smart watch full screen for iPhone and Android phones includes a bunch of new features including:The bluetooth smart watch can hang up the phone, receive and display WhatsAPP /Text /Facebook /Twitter /Messenger reminder.Support sedentary reminder, alarm clock, stopwatch, timer,weather information,music control, remote camera control compatible with Android 5.0 and above or iOS 9.0 and above smartphones.</t>
+  </si>
+  <si>
+    <t>imgamazon\71y5m2CJLUL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>Bluetooth Call and Message Reminders: After connecting to your phone via Bluetooth, you can answer/make clear calls directly from your fitness watch. You won't miss important calls when you don't have easy access to your phone, such as when you are running or driving. The fitness tracker also provides notifications of social media messages including Facebook, WhatsApp, Instagram, Twitter, etc. through vibrating alerts. Never miss any calls or messages again.
+1.96'' HD Screen &amp; 220+ Watch Faces: The fitness smartwatch is equipped with a large 1.96-inch HD colorful screen, delivering exceptional picture quality and highly responsive touch sensitivity. Provide you with better visual enjoyment. Customize your smartwatch with 220+ cloud-based watch faces or upload your own photos to express your unique style. Whether it's selfies or pictures of cherished moments, make your smart watch truly your own.
+24h All-Day Health Index Monitoring : The mens watch is equipped with the most advanced sensors. It can monitor your heart rate in real time throughout the day and you can view recorded data on the watch or App. Besides, the fitness smart watch tracks your sleep status automatically, including light sleep, deep sleep and awake time, helping you develop healthy sleep habits and improve sleep quality.
+113+ Sports Modes and IP68 Waterproof: The fitness tracker watch provides 113+ indoor and outdoor sports training modes to meet the sports needs of fitness enthusiasts, including: running, cycling, skipping, walking, mountain climbing, rock climbing, basketball, football, badminton, Yoga, dance and more. The IP68 waterproof design of the sports watch is not afraid of your sweating and hand-washing behavior, providing convenience for your daily life.
+Your Personal Smart Assistant: Smart watch for men women has a built-in large capacity battery, which can be fully charged in 1.5 hours, can be used for up to 7 days and has a long standby time of about 30 days. The smartwatches features practical tools such as stopwatch, timer, music control, weather, sedentary reminder, alarm clock, wrist up awake, etc, giving more convenience and fun to your life.</t>
+  </si>
+  <si>
+    <t>imgamazon\71jWH47R-DL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>Bluetooth Call and Message Reminders : This smart watch is equipped with an excellent chip processor. After connecting to your phone via Bluetooth, you can answer/make calls, view call history and store contacts through the smartwatch. The smartwatches also provides notifications of social media messages including Facebook, WhatsApp, Instagram, Twitter, etc. through vibrating alerts. Never miss any calls or messages again.
+24h All-Day Health Index Monitoring : The fitness smart watch is equipped with the most advanced sensors. It can monitor your heart rate in real time throughout the day, and can also automatically monitor your sleep status and analyze your sleep quality. In addition, it can also detect your step count, calories burned and more in real time. The data will be synchronized with the “GloryFit” application to generate health reports and suggestions to help you live a better healthy life.
+112+ Sports Modes and IP68 Waterproof : The fitness tracker watch provides 112+ indoor and outdoor sports training modes to meet the sports needs of fitness enthusiasts, including: running, cycling, skipping, walking, mountain climbing, rock climbing, basketball, football, badminton, Yoga, dance and more. The IP68 waterproof design of the smart watches is not afraid of your sweating and hand-washing behavior, providing convenience for your daily life.
+1.85" HD Touch Screen and 200+ Watch Faces : The smart watch is equipped with a 1.85-inch transparent glass screen, high-definition display, color reproduction, touch-sensitive, and not afraid of scratches. Provide you with better visual enjoyment. Through the “GloryFit” App, you can choose from more than 200+ watch faces styles. You can also customize your favorite photos as wallpapers in the fitness watch to meet your personalized needs.
+Long-Lasting Battery Life and More Functions : The smart watch uses a 280mAh large-capacity battery, which can provide 7 days of use, 30 days of standby time, and only takes 2 hours to charge. Smart watch are widely compatible with Android and iOS. It also provides a variety of practical functions such as stopwatch, timer, phone search, camera control, weather forecast, music control, breathing exercise, sedentary reminder, etc.</t>
+  </si>
+  <si>
+    <t>imgamazon\71er9UE84ML._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>2025 New Smart Watch with Bluetooth Call/Intelligent Notifications: The smart watches for men adopts bluetooth 5.3 version for a faster and more stable connection. With a built-in premium microphone and hd speaker, allowing you to answer calls and interact with voice assistants directly from smartwatch. Meanwhile, you can receive message notifications and read them from your watch, such as Facebook, Messenger, Instagram, Gmail, Whatsapp, Twitter etc. Just raise your wrist to view messages.
+1.96" HD Big Screen and Unlimited Customization Dials: smart watches for women adopt 1.96”TFT HD color display screen (320*386 resolution) which making it easy to operate and sensitive, experience crystal-clear visuals like never before. 4 level brightness adjustable allows you to read time and data clearly even under the glare. 200+ Multiple trendsetting combinations to match your mood and outfit of the day. Even create and customize your own mens smart watch faces from your phone gallery.
+24/7 Heart Rate Monitor and Sleep Tracker: Adopted high-performance optical sensors, Fitness tracker provides health monitoring features such as 24-hour continuity real-time Heart Rate, SpO2, and Sleep Monitoring(Deep/light sleep). It accurately monitors your heart rate in real time nd better understand your heart rate trends. Also, it provides a detailed analysis of your sleep quality and facilitating lifestyle adjustments by "GloryFit" continuously recording your sleep patterns.
+All Day Activity and Practical Functions: During exercise, sport smart watch automatically records daily steps, distance counter，calories burned, active minutes. This fitness watch men has other useful features offered like remote camera, music control, weather forecast, sedentary reminder, GPS tracking, stopwatch, find phone, raise to wake, alarm clock, calculator, etc. It makes things on your wrist simple and easy, and will always work as your effective daily assissant.
+110+ Multiple Fitness Modes and IP68 Waterproof: The waterproof watch supports 110+ sports modes indoors and outdoors (covering walking, cycling, hiking, yoga, etc). At the sametime, Connecting the GPS in your cellphone can track all your workout routes and physical status during exercise. The smartwtach men is IP68 waterproof, you can wear it when washing hands, in the rain(Note: Do Not use in showers, saunas, etc).
+30-day Standby Time and Wide Compatibility: The well-designed and detachable wristband which soft, lightweight, breathable and very comfortable when wearing. Beside, the android smart watch is designed with a large-capacity battery, Charging time is 1.5-2 hours，once charge which allows it to last about 5-7 days for daily use and 30 days on standby mode. P99 smart watches compatible with most android and iOS phone (andriod 6.0+ and iOS 10.0+).</t>
+  </si>
+  <si>
+    <t>imgamazon\711f6KLsMaL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>KEEP YOUR GOALS ON TRACK: Workout to your full potential with fitness tracking* on Galaxy Watch6; Get insights on duration, distance, calories burned and more; Watch recognizes activities from running to swimming and tracks over 90 other exercises
+FIND YOUR ZONE: Zone in on the results you want with personalized heart rate zones**; Watch scans your health data to provide HR zones tailored just for you; Target your preferred intensity to maintain the heart rate needed to achieve your goals
+SLEEP COACH ON YOUR WRIST: Get the insights to develop better sleep habits with Advanced Sleep Coaching*; Use Watch to plan your bedtime, detect snoring*** and understand and track your sleep stages (awake, light, deep, REM)
+ALWAYS-ON HEART MONITORING****: Your Watch continually scans your heart rate to inform you when it’s detected an irregular rhythm that might be A-fib — a heart-related abnormality that can lead to serious complications
+KNOW YOUR BODY INSIDE &amp; OUT: Stay in the know about your body with the advanced BIA sensor*****; Use your Watch to get readings on body fat, skeletal muscle, body water, Body Mass Index (BMI) and more*
+KEEP CONNECTED ON THE GO: Your Watch syncs with your other Galaxy devices seamlessly so you can play your favorite music, control your smartphone camera, make calls, text and do more from anywhere******
+OUR LARGEST WATCH DISPLAY YET: See even more on our largest display yet******* and quickly navigate apps thanks to an improved interface; Plus, durable crystal glass keeps screen looking great and protected from bumps and scratches
+MAKE MOVES IN STYLE: Match any mood or style with a wide variety of bands — now even easier to swap with one simple click********; Then accent your look with an assortment of new and enhanced Watch faces</t>
+  </si>
+  <si>
+    <t>imgamazon\71NclrgfIOL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>Bluetooth Call and Message Reminder: The mens smart watch are equipped with the latest Bluetooth 5.3 chip, which increases the connection speed by 80%, and a highly stable connection with no delay. Answer and make calls right from your wrist, and easily sync multiple mobile contacts. It also supports multiple smart reminders, including incoming calls, Email, texts, SMS messages (Facebook, WhatsApp, Twitter, Tiktok, Instagram, Gmail etc). You won't miss any important calls or notifications.
+1.91" HD Big Screen and DIY Dials: Fitness tracker features a TFT HD color screen (320 * 380 touch screen）and curved 3D curved glass for superior picture quality and touch sensitivity. Watch for men have more than 100+ unique online watch faces to choose from, you can also customize your watch face. It can be any photo, such as your family, star, pets, etc. Meanwhile, 4 levels manually adjust the brightness, so you can clearly see the displayed time and exercise data even in direct sunlight.
+110+ Fitness Modes and IP68 Waterproof: The fitness tracker watch provides up to 110+ sports modes, covering running, cycling, fitness and other activities to meet the preferences of different users. During your workouts, it will record data like heart rate, steps, calories burned, distance, and active hours in real time. The smartwatch for men is IP68 waterproof, allowing you to wear it during outdoor activities, rainy days, and while washing hands (Note: Do Not use in showers, saunas, swimming etc).
+24-Hour Health Activity Tracker: Smart watches for women track your Heart Rate, Blood Oxygen levels(SpO2) and Sleep patterns around the clock(deep sleep, light sleep, sleep quality analysis). And Your can track your period with menstrual cycle tracking and ovulation prediction as well. All data is presented in the "GloryFit" app, offering a comprehensive view of your health status. Watches women it is compatible with Android 5.0 and higher and iOS 9.0 and higher.
+30-day Standby Time and Multi-Functions: This smart watch for men has a large built-in 300 mAh battery that ensures up to 5-7 days of use and about 30 days of standby time with just 2 hours of charging. Sports watch also includes many utilities such as weather forecast, calculator, music control, camera control, alarm clock, sedentary reminder, stopwatch, timer, GPS, find your cell phone and more. Just enjoy your smart life by simply downloading GloryFit" for free from App Store or Google Play.</t>
+  </si>
+  <si>
+    <t>imgamazon\61H504jILXL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>Smart Watch for Seamless Connectivity: Stay connected with Bluetooth 5.3 for making calls and receiving notifications from messages and apps. With built-in Alexa, you can easily set alarms, control smart home devices, and more
+24/7 Comprehensive Health Monitoring: This smartwatch continuously tracks heart rate and blood oxygen levels with high-precision sensors. Automatic sleep tracking provides insights into your sleep patterns, helping you make informed decisions for a healthier lifestyle
+Accurate GPS Tracking: Enjoy precise location tracking with built-in GPS that connects to multiple satellite systems (GPS/GLONASS/BeiDou/Galileo). This feature allows you to monitor routes, distances, and pace without your phone, making it an ideal companion for outdoor workouts
+60+ Sports Modes for Every Athlete: Record daily activity metrics such as steps, calories burned, duration, and distance, empowering you to reach your fitness goals. The watch supports over 60 sports modes, catering to a variety of fitness enthusiasts
+Stunning AMOLED Display: The 1.78'' HD OLED display offers a maximum brightness of 1200 nits, ensuring clear visibility in all lighting conditions. The watch includes multiple functions such as customizable watch faces, alarms, weather forecasts, remote photography, and music control, making it a comprehensive tool for daily life and fitness tracking
+Long Battery Life &amp; Versatile Features: The 350mAh battery provides an average usage time of up to 7 days on a full charge. With a water resistance rating of 3ATM, this smartwatch is built to withstand the rigors of daily activities and outdoor adventures</t>
+  </si>
+  <si>
+    <t>imgamazon\61P1RD54mnL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>Bluetooth Call and Message Reminders: The smartwatch supports answering/making/hanging up calls, viewing call logs and storing contacts. The smart watch will vibrate to remind you of text messages, social media messages, such as Facebook, WhatsApp, Instagram, Twitter, etc. The smart fitness watch will give you real-time notifications, so you will never miss anything again.
+All-day Health Monitoring: The fitness watch has real-time health monitoring functions, which can monitor heart rate in real time; automatically monitor sleep status; test blood oxygen; do breathing exercises; all-day activity tracking steps, calories, distance, etc. The data will be synchronized with the "GloryFit" application to generate a health report.
+112+ Sports Modes and 200+ Dials: The smartwatch provides 112+ indoor and outdoor sports modes, such as running, cycling, skipping rope, walking, basketball, football, etc. You can switch dials on the smartwatch. In the "GloryFit" application, you also have 200+ dial styles to choose from, and you can also customize your favorite photos as wallpapers in the smart watch. There are also three menu themes to choose from.
+1.39" HD Touch Screen and Long Battery Life: The fitness tracker is equipped with a 1.39-inch round touch screen, large screen, high-definition display, color reproduction, sensitive touch, and scratch-resistant. The smartwatches can last for about 7 days in daily use and has an ultra-long standby time of about 30 days. It only takes 2 hours to charge with a magnetic charger.
+More Functions: The smart watches also has a variety of functions, such as: music control, weather forecast, remote photography, stopwatch, timer, alarm clock, find mobile phone, raise your hand to light up the screen, calculator, calendar, sedentary reminder, voice assistant, sound and vibration, flashlight, adjust brightness, do not disturb mode, etc. Download the "GloryFit" application to give you more intelligent experience.
+IP68 Waterproof and Wide Compatibility: The IP68 daily waterproof design of the smart health watch is not afraid of your sweating and hand washing behavior, providing convenience for your daily life. The fitness tracker watch is widely compatible with all iOS/Android smartphones, bringing you a convenient and pleasant experience.
+Give You the Ultimate Experience: Wearing this S51 - Smart watches give you a better experience. Multiple sports modes allow you to get a good partner for your sports/fitness, multiple health monitoring makes your life healthier, and multiple practical functions make your life more convenient.</t>
+  </si>
+  <si>
+    <t>imgamazon\71GtgMbKvKL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>ULTRA-BRIGHT AMOLED DISPLAY: With peak brightness of 2,000 nits, the Amazfit smart watch delivers easy reading of maps and workout data in any light. Night mode and Glove Mode enhance visibility for clear viewing
+DURABILITY FOR EXTREME CONDITIONS: This rugged smart watch, engineered with a 316L stainless steel bezel, withstands temperatures from -22°F to 158°F, and is water-resistant to 328 feet and can be used for freediving to a depth of 147 Feet
+EXTENDED BATTERY LIFE: The Amazfit T Rex 3 offers over 3 weeks of power with typical use or up to 180 hours in GPS mode, providing long-lasting performance for hiking trips or outdoor activities
+PRECISION NAVIGATION TOOLS: The smart watch for men and women provides free global maps with dual-band positioning. Six satellite systems offer fast, accurate GPS connections and precise turn-by-turn navigation
+EXPANSIVE FITNESS TRACKING: This fitness watch offers 170+ workout modes and AI-generated training plans, providing real-time updates to guide your fitness journey from hiking to surfing</t>
+  </si>
+  <si>
+    <t>imgamazon\71bSngCF5kL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>RUGGED DURABILITY: This rugged smart watch with a reinforced Generation 2 strap provides reliability and longevity. Ideal for running, swimming, cycling, gym workouts, hiking, and other outdoor sports
+COMPREHENSIVE FITNESS TRACKING: This tactical smart watch integrates with Adidas Running, Strava, Google Fit, Apple Health, and more, to provide detailed insights into your steps, distance, and calories burned
+PRECISE NAVIGATION: This iPhone and Android smart watch features five satellite systems like GPS and GLONASS for pinpoint navigation, ideal for smart watch users in hiking, hunting, and exploring
+EXTENDED BATTERY LIFE: With up to 16 days of regular use or 24 days with battery saver, this smartwatch for men or women allows uninterrupted focus on fitness goals without the need for frequent charging
+MILITARY-GRADE WATER RESISTANCE: Engineered for harsh conditions, this military smart watch handles swimming, cycling, and gym workouts with its 10 ATM water resistance and has passed military 7 grade tests</t>
+  </si>
+  <si>
+    <t>imgamazon\61k4v-fNKaL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>Health Monitoring Features: Track your heart rate and blood pressure 24/7, empowering you to stay proactive about your well-being. Dive into insightful sleep monitoring to optimize your rest for peak performance. Stay informed about your 02 levels for enhanced vitality. Plus, find moments of tranquility with guided breathing exercises, all from your wrist. Discover a smarter approach to a healthier lifestyle with FITVII fitness tracker.(Only for encouraging a healthy lifestyle, not for medical use)
+Fitness Tracking Capabilities: Elevate your fitness journey with FITVII fitness tracker's extensive tracking capabilities. Monitor your daily activities effortlessly, from steps taken to calories burned and distance traveled. With over 120+ sports modes, you'll find the perfect fit for your workout routine, whether you're hitting the gym or exploring the great outdoors.
+Convenient Reminders: Stay on track throughout your day with FITVII smart watch reminders. Avoid prolonged periods of inactivity with sedentary reminders and stay hydrated with drinking water reminders. Women's health feature tracks your menstrual time and record menstrual changes to learn more about your body. Never miss an appointment with our alarm clock feature, keeping you punctual and organized.
+Handy Bluetooth Features: FITVII fitness watch goes beyond health and fitness, offering a range of convenient features. Built-in AAC Audio Technology, enjoy crystal-clear Bluetooth calls directly from your wrist. Receive texts and app notifications, locating your misplaced phone has never been easier. Enjoy your favorite tunes on the go with Bluetooth music playback control, and capture memories effortlessly with remote camera control, all from the convenience of your wrist.
+Practical Utility Features: Experience convenience at your fingertips with FITVII smartwatch's array of practical functions. Stay ahead of the weather with real-time forecasts delivered directly to your wrist. Whether you're timing laps at the track or tracking your workout, our stopwatch and countdown timer ensure precision. Keep your schedule organized with easy access to your calendar. Stay connected with quick access to your contacts. Need to crunch some numbers? Our built-in calculator has you covered.
+Water resistant Design and Durability: Designed to withstand your active lifestyle, FITVII smartwatch features a IP67 water resistant, allowing you to wear it with confidence rain or shine. (Not suitable for diving or surfing)
+Long Battery Life &amp; Compatibility: With a battery life of up to 7 days(Varies with use and other factors). FITVII fitness tracker seamlessly syncs with Android 5.1 / iOS 10.0 and above smartphones with 5.0 Bluetooth (Not for PC or tablet)</t>
+  </si>
+  <si>
+    <t>imgamazon\71oaX1N6STL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>⌚【1.85'' HD Color Touch Screen and Personalized Style】The fitness smart watch is equipped with a 1.85'' high-resolution HD touch screen, bringing you an unprecedented use experience. This smart watch has more than 100 unique watch faces to choose from. You can also customize your favorite pictures as watch faces on ‘’Da Fit‘’ APP, or customize your favorite wallpapers, giving you a unique experience every time you check the time.
+📞【Making/Receiving Calls and Voice Assistant】The smart watch has a built-in speaker and microphone, and after connecting to your phone via Bluetooth, you can activate the AI voice assistant to issue commands. For example, make calls, control music, check the weather, set alarms and timers, etc. When your phone receives a call or message (such as WhatsApp, Facebook, Instagram, etc.), the smartwatch issues a real-time notification, making you never miss anything and making your life more convenient and better.
+🏃【More Than 100 Sports Modes】This fitness watch provides more than 100 sports modes: running, basketball, yoga, cycling, walking, climbing, badminton, tennis, etc. You can also view your complete workout data in the ‘’Da Fit‘’ APP. The watch automatically records your daily steps/calories/exercise distance, etc. As well as a timer, stopwatch, and other functions to help you exercise. You can also set exercise goals (Like almost all non-GPS smartwatches, this watch counts your steps based on your arm movements. So if you move your arms like normal while running, the watch will be more accurate to count your steps.)
+💓【24/7 Health Monitoring】The fitness pedometer watch is equipped with a motion sensor that can automatically monitor dynamic heart rate in real-time 24/7, It can also track personal sleep and detect blood oxygen saturation and stress to adjust the personal physical condition. Offer a detailed sleep quality analysis report (light sleep/deep sleep/awake stage) through the App, helping you adjust your lifestyle and healthier. This smartwatch also helps women track their menstrual cycles.[NOTE: This watch can't be used as a medical diagnostic tool.]
+👍【More Features, More Fun】The men women's smart watches also have other useful daily functions, such as smart notifications, music control, camera control, casual games, weather forecast, sedentary reminder, alarm clock, stopwatch, timer, etc., and wait for you to dig. The step counter watch is compatible with Most Android 6.0 and iOS 9.0 or above smartphones. Built-in large capacity battery - 300mAh, up to 5 days of use and approximately 30 days of standby with just 2 hours of charging.
+⚠【Note】① Since the watch is equipped with speakers and microphones, therefore it is not recommended that you take the watch to swim or dive. But the smart watch fully meets daily dustproof needs such as hand washing and sweating, ② We provide a long after-sales period and very complete customer service, If you need help using your smart watch, please do not hesitate to contact us immediately. We will reply to your message within 24 hours and help each customer solve all problems quickly.
+❗Note: The case and strap of our smartwatch are "FSC-Certified".</t>
+  </si>
+  <si>
+    <t>imgamazon\71uSftQvyZL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>Easy-to-use running smartwatch with built-in GPS for pace/distance and wrist-based heart rate; brilliant AMOLED touchscreen display with traditional button controls; lightweight design in 43 mm size
+Up to 11 days of battery life in smartwatch mod and up to 19 hours in GPS mode
+Reach your goals with personalized daily suggested workouts that adapt based on performance and recovery; use Garmin Coach and race adaptive training plans to get workout suggestions for specific events
+25+ built-in activity profiles include running, cycling, HIIT, strength and more
+Download songs to your compatible watch, including playlists from Spotify, Amazon Music or Deezer (subscription required), and connect with your wireless headphones for phone-free listening
+As soon as you wake up, get your morning report with an overview of your sleep, recovery and training outlook alongside weather and HRV status (data presented is intended to be a close estimation of metrics tracked)
+With training effect and training effect labels, you’ll see how your workouts impact your fitness and understand the primary benefit achieved from your workout; recovery time lets you know how long you need to recover before your next high-effort workout
+Safety and tracking features, including incident detection (during select outdoor activities) and Assistance, send a message with your live location to emergency contacts when paired with your compatible smartphone; requires setup and your smartphone to be in an area with network coverage where data connectivity is available
+Never miss a call or text with smart notifications from your paired Android or Apple smartphone
+Leave your cash and cards at home; Garmin Pay contactless payments let you pay for purchases on the go (with a supported country and payment network)</t>
+  </si>
+  <si>
+    <t>imgamazon\61OgsMROcPL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>Smartwatch for Women/Man</t>
+  </si>
+  <si>
+    <t>imgamazon\7118sA6NB3L._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>Make/Answer Call &amp; Read Message: Bluetooth call smartwatch is equipped with built-in HD speaker, after connecting to your android/iOS phones via bluetooth, you can answer or make calls, store emergency contacts and view call history through directly use the smart watch; The mens smart watch can also receive notifications from apps including Facebook, WhatsApp, Instagram, Twitter, SMS, etc. So that you will never miss any important information
+2.0" HD Color Screen &amp; 100+ DIY Dial: Smart watches for men women is equipped with a 2.0" extra-large hd full touch color screen, clear picture quality and high touch sensitivity; In the "Da Fit" app, you can download more than 100+ watch faces for your fitness activity tracker smartwatch, or design upload personalized photo and set it as your desktop for android/ iphone smart watch
+Personal Health Steward: The health monitoring smartwatch adopting advanced sensors, 24-hour a day monitors your heart rate, blood oxygen and sleep. you can more understand your real-time heart rate, blood oxygen saturation and sleep status(deep/light/wakeful sleep) by our fitness tracker watch, to make you understand your physical health through this smart watch for android phones
+100+ Sports Modes Activity Fitness Tracker: This fitness watch for men women supports multiple sports modes, including running, hiking, cycling, skipping, walking, basketball, yoga, football and more. Activity trackers and smartwatches will record your data like heart rate, steps, calories burned, etc during your exercise; IP68 waterproof design of the sports watch perfectly meets your daily waterproof needs, But it is not recommended for use in hot water, seawater, swimming, diving or bathing
+30 Days Standby Time &amp; Multifunction Smartwatch: Smart watch for men has multiple functions such as timer, stopwatch, alarm clock, find your phone, sedentary reminder, music control, weather forecast, do not disturb mode, brightness adjustment, camera control, female cycle tracking; The smart watch for iPhone compatible charging for 2 hours, 5-7 days of normal use and 30 days of standby time. This android/iPhone watch for men is compatible with smartphones with Android 5.0 and iOS 9.0 or above</t>
+  </si>
+  <si>
+    <t>imgamazon\61IZmXci7qS._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>BODY COMPOSITION ANALYSIS: Galaxy Watch4 is the first smartwatch to off body composition data right on your wrist, On your own schedule, now you can get readings on body fat, skeletal muscle, body water, basal metabolic rate, and Body Mass Index.Supported Application:Heart Rate Monitor,Sleep Monitor,Fitness Tracker. Connectivity technology:LTE,Bluetooth,GPS. Wireless comm standard:Bluetooth
+BETTER SLEEP STARTS HERE: Wake up feeling refreshed and recharged with advanced sleep tracking; When you go to bed, your Galaxy Watch4 sleep tracker starts monitoring your sleep and SpO2 levels continuously
+BE SMART ABOUT YOUR HEART: Take care of your heart with accurate ECG monitoring and keep an eye on possible atrial fibrillation, a common form of irregular heart rhythm; Share personalized readings with your doctor using the Samsung Health Monitor app on your compatible Galaxy phone
+MAKE EVERY WORKOUT COUNT: Get the most out of every exercise session with advanced workout tracking that recognizes 6 popular activities, from running to rowing to swimming, automatically in just 3 minutes; Stay motivated by connecting to live coaching sessions via your smartphone or to dynamic Group Challenges with your friends
+GO THE EXTRA MILE: Improve your runs with advanced running coaching technology; VO2 Max readings assess your oxygen levels to manage and track your heart and lung endurance
+EXTENSION OF YOUR PHONE: Put the phone features you need right on your wrist and stay connected to calls, texts, notifications, and music streaming, all accessible with a simple tap
+GOOGLE ON YOUR WRIST: Tap into the power and convenience of select Google services and apps right from your wrist; Pay for coffee; Get directions to the park; Use Bixby or Google Assistant for help on almost any topic; Stream your favorite tunes on YouTube</t>
+  </si>
+  <si>
+    <t>imgamazon\61d46oYQgdL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>BIG SCREEN. FAMILY-SIZED FUN: Bring fun home to everyone with a bright, engaging screen; great for videos, games or fun time for the kids (11” 1920 x 1200, 90Hz, 480 nits, TFT LCD)
+RICH SOUND ALL AROUND: Your music; Your shows; Your games; Hear them all loud and clear, thanks to quad speakers powered by Dolby Atmos; Galaxy Tab A9+ delivers a cinema-like audio experience your ears will love
+POWER FOR ALL YOU DO. STORAGE FOR ALL YOU LOVE: Watch videos, play games and do more with an upgraded chipset; 4GB RAM + 64GB | 8GB RAM + 128GB | Up to 1TB expandable storage; Processor Qualcomm Snapdragon 69
+SEE and USE MULTIPLE APPS AT ONCE: Open multiple apps at once with Galaxy Tab A9+ and accomplish more seamlessly; Bounce between the things like a multitasking pro — browse the internet, check email and jot down notes all on one screen
+LOVED BY KIDS. TRUSTED BY PARENTS: Give your kids a safe place to learn and play with the Samsung Kids app⁵ ; Kids will love a wide variety of playful, colorful content that keeps them entertained while stimulating their young minds
+SLIM. LIGHT. DURABLE: Carry your Tab easily with a slim, light design that’s also durable; Galaxy Tab A9+ is the perfect blend of performance and portability to help you bring the fun with you wherever you go
+SEND FILES IN A FLASH: Sharing files has never been easier with Quick Share⁶ ; Select the file you want to share on your device —from a video clip to a photo, then easily transfer the file to another device whether it’s Android or iOS
+TAKE IT TO THE BIG SCREEN: With Smart View, experience videos exactly how you want; Looking to see more detail on a sports clip or cooking video you’re watching on your Tab Cast it to your Samsung TV and experience the thrills on your TV screen⁷
+KEEP THE CONVERSATION GOING: With Galaxy, it’s easy to stay connected to family and friends; Pick up a call or return a text from your Tab⁸ , even if your phone is in the next room
+For manufacturer contact information, please visit the official website, accessing the link in the "Visit the SAMSUNG store" section, right under the item title</t>
+  </si>
+  <si>
+    <t>imgamazon\71cAVmsvgjL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>【High Performance】URAO Android tablet features the latest operating system Android 14 and an 2.0 GHz octa-core processor ensure of excellent performance, seamless multitasking, getting rid of annoying ads, emphasizing privacy and security by designing enhanced app permissions, providing you complete management control.
+【Massive Storage 】Our Android tablet comes with 10GB (4+6GB) RAM 128GB ROM and maximun 1TB TF card ( not included )expandable ensures you of a fast APP launch and smooth gaming experience. URAO tablet also come with pre-installed Google Play Store, you can easily download any needed Apps such as Netflix, Facebook, Twitter, Youtube, etc.
+【HD Eyes Protection Display】URAO tablet equipped with a high resolution 1280*800 IPS display, which shows a brightly colored wide-screen for a more realistic viewing experience with sharper and brighter images.The front 5MP and rear 8MP cameras can easily satisfy video calls, online learning, etc. The tablet LCD designed with low blue light technology, the screen flicker and the damage to the eyes caused by irritating blue light will be reduced.
+【Large Capacity Battery with Fast Charge】The built-in large capacity and low consumption CPU enable our URAO 10 inch tablet to stand by for up to 3 days and allows you to enjoy up to 8 hours of mixed reading, watching TV shows, playing games, surfing the web. URAO tablet dopts fast-charging technology which can be fully charged in 1.5 hour and easily charge via the USB Type-C port and rest assured the battery will last. It is a good companion for you to play and study!
+【Wi-Fi 6+Bluetooth5.0】URAO android tablet 10 inch adopts the lastest sixth generation WiFi technology and the upgraded bluetooth 5.0. Dual band integrated chips make the 5g WiFi and 2.4g WiFi more stable and the lastest bluetooth 5.0 connection supports all your favorite accessories, highly increased the speed of data transfer, improved network capacity and reduced network delays.
+Note:The tablets have no GPS; tablet is based on Android system , cannot directly share accounts with IOS system.</t>
+  </si>
+  <si>
+    <t>imgamazon\617tvSqW30L._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>【Latest Android Tablet】- This android tablet features a quad-core processor, android 13 OS and a 10.1" IPS screen, its smooth operation enables seamless video playback, gaming, and multitasking.
+【6GB RAM/64GB ROM + 1TB Expand】- With ample storage capacity that can be expanded up to 1TB via SD card (sold separately), you can confidently store all your photos, videos and files without concerns.
+【IPS Display &amp; Dual Camera】- Equipped with 10.1" IPS 1280x800 HD screen, 2.0MP front camera/8.0MP rear camera, this android 13 tablet offers you a delightful experience while watching movies, reading books, or making video calls.
+【Long Battery Life】- Built-in 6000mAh lithium battery, this android tablet provides up to 8 hours of uninterrupted video playback, enabling you to use it for longer periods without any interruptions.
+【Worry-Free Service】- We offer comprehensive support to put your mind at ease. Our warranty lasts for 1 year. If you have any questions, please don't hesitate to contact us. We will respond promptly and assist you in resolving any issues.</t>
+  </si>
+  <si>
+    <t>imgamazon\71XySfAlGuL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>The Pixel Tablet is helpful at home and with work; it features Google AI for smooth streaming, high-quality video calls, and more
+The 11-inch screen with brilliant colors and adaptive brightness is perfect for streaming shows and movies and editing photos and videos[1]; and multitasking is easy with Split Screen[10]
+Google AI helps with everyday tasks; search anything right from the app you’re in, just by drawing a circle around an image, text, or video[15]; and Magic Editor makes photo editing easy; AI can change the background, move objects, and more[16]
+Kickstart your productivity and creativity with Gemini; brainstorm ideas, write notes, make plans, and more[2,17]
+Manage your smart home devices with your voice or a tap on the home panel; access and adjust your compatible thermostats, lights, locks, and cameras[4]
+The Android apps you love are optimized for your Pixel Tablet’s larger screen; watch shows and movies with Google TV[5] and cast content with Chromecast built in[6]; a Charging Speaker Dock (sold separately) is required to initiate casting
+Securely share photos, videos, and more between your Pixel Tablet and other nearby phones and laptops with Quick Share[7]
+It works seamlessly with other Google Pixel devices; effortlessly connect your Pixel phone, earbuds, watch, and tablet with each other[8]; and easily switch audio between your Pixel phone, earbuds, and tablet[9]
+The Pixel Tablet comes with Google Meet for HD video calling; the camera follows you so you can move around the room while staying in frame, and automatic lighting adjustments keep you looking your best
+Please refer to the “Legal” section below for all applicable legal disclaimers denoted by the bracketed numbers in the preceding bullet points (e.g., [1], [2], etc.)</t>
+  </si>
+  <si>
+    <t>imgamazon\61Sna00l0tL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>✅【Latest Android 14 Tablet】Eksvefot tablet comes with a powerful Android 14 system, which brings you a whole new task bar and a more user-friendly UI with enhanced customization options. Android 14 also emphasizes privacy and security by designing enhanced app permissions, giving users complete management control and offering heightened security measures. The update of PC mode also brings you more convenient operation and you can use Face ID to unlock tablet.
+✅【Smoother Sensitive Experience &amp; Fast Connection】The android tablet is equipped with a powerful A55 architecture and an Octa-core CPU, delivering a smooth and fast performance and convenient operations. Capable of supporting a maximum frequency of 2.0GHz, use a low-power 22nm process for lighter operation and faster processing with lower heat and power consumption. Whether you're watching videos, browsing the web, or listening to music, you will enjoy a seamless and uninterrupted experience. This 10" tablet effortlessly handles multitasking and demanding applications.
+✅【2025's Latest Memory Version】 This 10-inch tablet comes with 10 (3+7) GB RAM, 64GB ROM and a micro-SD card slot that allows for an expansion of 1TB of memory. Large and expandable storage can run more smoothly and you can quickly launch applications and enjoy it without the stress of running out of storage space. Feel free to download any app you want. Our tablet also come with pre-installed Google Play Store, you can easily download any needed Apps such as Netflix, Facebook, Twitter, etc.
+✅【10.1-inch IPS &amp; Long-Life Battery】The tablet android equipped with a high resolution 1280*800 IPS display, which shows a brightly colored wide-screen for a more realistic viewing experience with sharper and brighter images. Comes with a 3-layer screen protector which prevent screen scratches. This 10-inch android tablet also equipped with a rechargeable battery up to 5000mAh, it lasts for up to 8 hours on a single charge. You can also use the Type-C port to connect mouse and keyboard. Allow you to work or play all day while you're on the road.
+✅【Perfect Gift &amp; Dynamic Halo】The android tablets with lightweight and slim design, which allows you to enjoy e-books, movies, TV shows and music effortlessly while traveling or on business trips. We provide a one-year warranty for the A10 Android 14 tablet. If any quality issues arise, please contact us through your Amazon purchase records and we will work to ensure customer satisfaction.</t>
+  </si>
+  <si>
+    <t>imgamazon\616SXS5m0eL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>BIG DREAMS CALLING - The Lenovo Tab P12 puts the fun in functional with next-level, detailed visuals and 3K resolution that's helpful for taking notes in class and winding down with immersive gaming after schoolwork is done
+EXPANSIVE ENTERTAINMENT - Enjoy some well-deserved downtime with the vibrant visuals of a 12.7-inch LCD screen with up to 1080p streaming quality, enhanced by quad speakers with Dolby Atmos surround sound
+GET YOUR GAME ON - Finish homework quickly and revel in uninterrupted, fast-paced gameplay with a Wi-Fi 6 connection, MediaTek Dimensity 7050 Octa-Core processor, 8 GB LPDDR4x RAM, and 128 GB Universal Flash Storage
+CAPTURE THE MOMENT - An ultra-wide front-facing 13MP camera, AI face tracking, and RGB sensor keeps the focus on your face and movements during video calls and recordings
+SPLIT SCREEN PRODUCTIVITY - The 16:10 aspect ratio screen has plenty of room for 4 split screens letting you write, play, and perform simultaneously
+SMART LEARNING FOR SMART MINDS - Draw, edit, and structure your note taking with the included Tab Pen Plus that has built-in tilt detection, palm rejection for accurate strokes, and a helpful lost connection alert
+ESCAPE REALITY WITH FICTION - The Tab P12 customizes your color display with chromatic or mono modes, and has a selection of 20 background songs, curated to pull you deeper into your imagination while you read
+EQUIPPED FOR SCHOOL AND ENTERTAINMENT - Connect your accessories and other devices with the 1 USB Type-C 2.0 port and 1 Micro SD slot, protected with included folio case for safekeeping
+SIZE (D x H x W) - 6.9 (8.42 with camera bump) x 190.76 x 293.37 mm or 0.27 (0.33 with camera bump) x 11.55 x 7.51 inches
+INCLUDED ITEMS - Tablet, Pen, Grey folio case, USB Type-C 2.0 charging cable, 20W charging adapter, Quick Start Guide &amp; Safety, Warranty, MicroSD tray pin</t>
+  </si>
+  <si>
+    <t>imgamazon\71x3Cq4C8VL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>RAPID AND POWERFUL SYSTEM: The tablet has the latest Android 14 system and an octa-core processor, which provides excellent performance, seamless multitasking, and enhanced privacy features. Its user-friendly interface makes it easy to navigate and split-screen functionality allows you to adapt seamlessly to your digital lifestyle.
+AMPLE MEMORY &amp; ROBUST BATTERY CAPACITY: The Android 14 tablet comes with 8(4+4)GB RAM and 64GB storage space, which can be expanded to 512GB via TF card, allowing you to download movies, e-books and music, ensuring you have enough space for your files. The 5000mAh battery provides up to 6-8 hours of uninterrupted use,ensuring reliable performance throughout your day.
+IPS DISPLAY &amp; SPILT SCREEN: The tablet features a 10.1-inch IPS display with 1280x800 resolution for an immersive viewing experience. With its split-screen feature, you can open 2 apps at once, improving efficiency and workflow, and helping you complete tasks, meetings, and presentations in no time.
+GMS CERTIFICATION: The tablet is GMScertified, providing seamless access to a host of apps and services. Easily download Facebook, Twitter, YouTube, TikTok, Line and Instagram.
+WORRY-FREE WARRANTY: Tablets come with a 1-year warranty and lifetime technical support. Should you have any inquiries regarding your tablet, don't hesitate to reach out to us via Amazon email. Rest assured, our dedicated team will address your questions promptly within 24 hours.</t>
+  </si>
+  <si>
+    <t>imgamazon\417bx91cc8L._AC_SL1000_.jpg</t>
+  </si>
+  <si>
+    <t>CIRCLE IT, SEARCH IT, FIND IT. JUST LIKE THAT: Search for anything you see on your Galaxy Tab S9 FE Series screen simply by circling it. From discovering where to buy those awesome shoes to getting a recipe based on a dish your friend just posted, find answers fast using Circle to Search with Google.¹
+A SCREEN FOR ALL YOUR ADVENTURES: Start every adventure with a large, beautiful 10.9" screen. Whether you’re a multitasker, a gamer or a devoted movie watcher, you’ll feel closer to the action. Plus, dual speakers make everything sound amazing
+BUILT FOR ADVENTURE: An IP68 rating makes Galaxy Tab S9 FE one of the only water- and dust-resistant tablets on the market. It’s built to last wherever you use it, making it a great choice for first-time tablet buyers
+A BATTERY THAT KEEPS YOU IN CHARGE: With a tablet this powerful, portable and fun, you’ll never want to put it down. Go up to 18 hours with a long-lasting battery and get a full charge in less than 90 minutes with Super Fast Charging
+POWER FOR ADVENTURE: The latest Exynos chipset lets you own the day and stay in touch. Cross off your to-do list and video chat with your college roomie miles away. Whatever you’re doing, Galaxy Tab S9 FE makes for rich experiences
+SMART TECH, BEAUTIFULLY MADE: Galaxy Tab S9 FE complements your personality perfectly. Plus, with a refined design that’s sleek and lightweight, you’ll be able to show off your great taste anywhere you use your Tab
+PEN-POINT PRECISION: There’s virtually no limit to what you can do with S Pen. Write notes by hand. Draw a comic strip or mark up a document. Pen features a responsive design that feels like you’re writing on actual paper
+STORAGE FOR ALL YOUR ADVENTURES: Life’s an adventure, so keep track of your favorite moments with up to 256GB of storage. That’s plenty of space and if you need more room, add up to 1TB more with a microSD card
+CAMERAS BUILT FOR VIDEO CHAT: Collaborate effortlessly with a camera that automatically adjusts to keep the focus on you. Plus, with a large display that opens up to 3 apps at once, you can multitask while you video chat.
+FILE SHARING MADE EASY: Sending and receiving files is so easy with Quick Share. From selfie videos to large work files, transfer to and from your Galaxy Tab S9 FE in a snap — it even works when sending to non-Galaxy devices</t>
+  </si>
+  <si>
+    <t>imgamazon\618mxQZWt1L._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>Chill for a longer time: Binge, chill and relax with a 5100 mAh battery that offers up to 13 hours of video playback
+Immersive Cinematics: Watch your favorite movies and shows on a 9” HD display for a stunningly mobile cinematic experience
+Search what you see with Google Lens: Translate text, get help with homework, or quickly identify products, plants and places with Google Lens
+Keep your security on lock: Keep your tablet’s security under lock and key with facial recognition for safe and convenient log-in
+Power Play: With a powerful MTK G80 Octa Core processor and up to 32GB of storage, gaming and browsing is smooth and fun</t>
+  </si>
+  <si>
+    <t>imgamazon\71sut5qBVsL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>【Android 15.0 tablet】 CUPEISI tablet adopts the 2025 latest version of Android 15.0 system and has passed Google GMS certification, The android 15 tablets offer personalized security systems, lightning fast application launches, super smooth gaming, and stunning netflix multimedia experiences.
+【18GB RAM+128GB ROM+2TB Expandable】 The Android 15 tablet PC built-in a powerful storage combination of 18GB RAM (6GB + 12GB achieved through expansion technology) and 128GB ROM, comes with new generation ultra-high performance and low power consumption 2.0GHz CPU, achieve faster and more stable running and storage speeds. In addition, it can be expanded up to 2TB with a microSD card (card not included) for even more storage.
+【Portable 2 in 1 Tablet with Keyboard】 This 10.1 inch Android 15 tablet equipped with a bluetooth keyboard, wireless mouse, and stylus as well as a foldable protective case, allowing you to seamlessly transform your 10'' tablet into a laptop-style device. This versatility makes it the ideal device for those who need to be productive on the go, whether it be for work, study, or play.
+【10.1 inch Touchscreen &amp; HD Camera】 The android 15.0 tablet has a 10.1 in IPS display, 1280x800 resolution, a tablet with sensitive screen sensing, equipped with 8MP+2MP HD cameras, narrow edge screen design. The high-definition screen brings you more detailed natural colors and advanced visual effects. The "reading mode" can reduce harmful light to the eyes so you get to enjoy a comfortable night reading.
+【2.4G/5G Wi-Fi 6.0+6000mAH Battery】 10 inch Wifi tablet support 5Ghz Wi-Fi 6 or 2.4Ghz, it has a more stable wireless signal, achieves faster transmission speed, and makes wireless devices more power-saving. In addition, it is equipped with a 6000mah battery, a single charge can last up to 10 hours, perfect for long-distance commuting and travel, reading, watching movies, dramas, listening to music and so on.</t>
+  </si>
+  <si>
+    <t>imgamazon\81r0y-Pg1lL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>2025 Latest Android 14 Tablet - The latest Android 14 OS represents a significant upgrade in speed, security, and user experience. Android 14 tablet include enhanced performance and efficiency and predictive functions, optimized multitasking capabilities, and a refined user interface that enhances overall usability and customization options. Android 14 Tablet has been certified by play store, any apps in play store you can get easily.
+Powerful Performance &amp; Large Storage - Experience seamless multitasking and fast app launches powered by a powerful octa-core processor, ensuring swift app launches and smooth operation. 10GB RAM (4GB + 6GB expand) - The android tablet with 64GB internal storage and expandability up to 1TB via microSD card. Store your apps, photos, and files effortlessly with generous internal storage options, providing ample space for your needs.
+Long Battery Life - Android tablet boasts a 6000mAh -Lasting battery, enjoy extended usage sessions with a high-capacity battery that keeps you powered throughout the day(8-12Hours), ideal for work or entertainment on the go. Stay connected with dual-band WiFi and optional 2.4/5G support, ensuring fast internet speeds wherever you go.
+High-Resolution Display &amp; Enhanced Connectivity - Immerse yourself in vivid detail with a high-resolution 10.1 -inch screen, perfect for movies, games, and productivity tasks. Enjoy blazing-fast internet speeds with dual WiFi support (2.4GHz + 5GHz) and WiFi 6 compatibility, ideal for streaming, gaming, and browsing without interruptions.
+Capture Every Moment &amp; Dual speakers- Capture stunning photos and videos with the 2MP front-facing and 8MP rear-facing cameras, perfect for video calls, selfies, and documenting your adventures. Stay connected and productive with Bluetooth 5.0 technology, ensuring seamless pairing with wireless devices for enhanced versatility and convenience. Dual speakers are designed to provide high-quality and powerful sound for your favorite music, games and videos.</t>
+  </si>
+  <si>
+    <t>imgamazon\71aUuA8F3XL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>【Android 14 tablet, 128GB ROM】2024 new large-capacity Android 14 tablet 10.1 inch K50 has 10GB RAM (4GB RAM + 6GB extend), 128GB ROM allows you to store more photos and documents. A micro SD card slot expands storage up to 1TB, so you can store all your favorite media files together, including ebooks, videos, photos. The 10.1 inch tablet with Android 14 and GMS certified, allowing you to download popular apps from the Google Play Store.
+【FHD IPS Display】The tablet equipped a FHD IPS 10.1" display with a resolution of 1280*800, It provides you a bright display and vibrant colors for a more realistic viewing experience. Ensure smoother motion in movies .FHD IPS 10.1" display is good for eye protection during use.
+【Multi-functional 10 inch tablet】 6000mAh+Type-C+3.5mm headphone jack, Large-capacity battery enables long-term use when traveling. you can work and entertain at the same time.Moderate weight, making it easy for you to take with you to work, study, or on the go. The tablet has a built-in 8MP rear camera and 5MP front camera, which can meet your daily video call needs. You can also use it to shoot videos and record your daily life.
+【Dual-band WIFI &amp; Bluetooth 5.0】 The tablet supports dual-band 2.4G/5G high-speed Wi-Fi, with the 5G band offering faster speeds and a less disruptive internet experience. This tablet strong network speed can greatly improve work efficiency and improve gaming experience and meets reading, photograph, videos, music, etc. suitable for most life scenarios.
+【Multi-functional and thin 10.1 inch tablet】The K50 tablet is equipped with 2 sound chambers to bring you a better external listening experience. The K50 is 7.7mm, It weighs 530 grams, making it easy to carry with you to work, study or on the go.</t>
+  </si>
+  <si>
+    <t>imgamazon\81o3TO8tqbL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>2025 Android 14 operating system - 10 inch tablet is equipped with the android 14 system. The new system improves privacy and data protection and makes it faster and more secure. The system fully protects user privacy and offers extensive personalized settings
+10GB RAM+64GB ROM+1TB Expandable - Android 14 tablet PC integrates a powerful memory combination of 10GB RAM (4GB+6GB achieved by expansion technology) and 64GB ROM with support expansion to 1TB for SD card. The extremely large RAM provides plenty of space to run apps as well as download and save photos, movies and games
+Ultra High Performance Octa-Core CPU and Large Capacity Battery - Powerful tablet comes with the new generation ultra-high performance and low power consumption Octa-Core 1.6GHz CPU, achieve faster and more stable running and storage speeds. Equipped with a 6000mAh high capacity battery, provides enough power to run the tablets
+Enjoy more functions - Android tablet supports 5G and 2.4G dual-band Wi-Fi, more stable WiFi signal for wireless devices, faster transmission speed and more energy saving. The tablet has built-in bluetooth 5.0 function, which is more stable and faster. You can connect bluetooth devices such as bluetooth headphones, bluetooth keyboard, etc. Plus, the 10 inch IPS HD screen, has a super high resolution of 1280 x 800, Equipped with a clear 5 megapixel front camera and 8 megapixel rear camera, record every moment in your life
+Ideal choice for family - The tablet has excellent performance, friendly design and elegant packaging, making it a perfect choice for Christmas, Valentine's Day, birthdays. Our tablets have features such as digital wellbeing and parental controls so you can set screen time limits, security modes and content management</t>
+  </si>
+  <si>
+    <t>imgamazon\71quWoCtTgL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>【ULTIMATE ANDROID 13 &amp; OCTA-CORE &amp; 2.0 GHZ】Tablet S22 is equipped with the latest Android 13 system, which enhances privacy and security for better privacy protection and data control. The tablet is equipped with the most stable octa-core processor with a maximum frequency of 2.0GHz, which improves program running speed and mobility for web browsing, bringing a faster user experience.
+【12GB RAM + 128GB ROM + TF 1TB 】Tablet 10 inch offers 12GB RAM（6GB RAM + 6GB RAM expansion） and 128GB storage, compatible with all brands of microsd/TF cards from 4GB to 1TB. The 12GB memory allows you to launch apps quickly, and the large memory allows you to enjoy millions of movies and TV shows, bringing you a more convenient and smooth user experience.
+【5G/2.4G WiFi + Bluetooth 5.0】Android 13 tablet support 5G Wi-Fi, New WiFi receiving and transmitting channels improve the speed and stability of network connections. Suitable for all home networks.Connect Bluetooth headsets, Bluetooth keyboards and other Bluetooth devices via Bluetooth 5.0. The tablet is GMS certified and offers full access to a wide range of Apps to download the apps you need.
+【DISPLAY + CAMERA + FACIAL RECOGNITION】Tablets feature a 10-inch 2.5D IPS 2.5D touch screen with 1280*800 HD resolution with color reproduction and brightness.The S22 comes with dual cameras: a 5-megapixel front and an 8-megapixel rear camera. Not only can you video chat with your family, friends and colleagues through the app, but you can also unlock the screen via facial recognition.
+【TABLET 2 IN 1】 Tablet with mouse and keyboard can be used as small laptops.The tablet also includes adapter, case, charger, screen protector and more. We offer lifetime technical support and lifetime. If you have any problem during use, please feel to contact us through Amazon. We will have professional staff to help you solve the problem.</t>
+  </si>
+  <si>
+    <t>imgamazon\61swRiNn7vL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>High-Performance 10 Inch Android 14 Tablet: Boost your productivity and entertainment with this 10-inch Android 14 tablet, featuring a powerful 2.0 GHz Octa-Core processor and 12GB RAM. Enjoy seamless multitasking, faster app launches, and enhanced privacy with advanced app permissions. This Android tablet is designed to deliver a smooth, experience while keeping your data secure.
+Massive Storage with 64GB ROM: This 10-inch tablet comes with 64GB of internal storage, expandable up to 1TB via a TF card (not included). Store all your apps, games, and media effortlessly. Pre-installed with Google Play Store, you can easily download popular apps like Netflix, YouTube, Facebook, and more.
+HD Eye Protection Display &amp; Dual Cameras: Immerse yourself in vibrant visuals on the 1280x800 IPS touchscreen display. Designed with low blue light technology, this 10-inch Android tablet reduces eye strain, making it perfect for extended use. Capture every moment with the 2MP front and 5MP rear cameras, ideal for video calls, online learning, and more.
+Long-Lasting 6000mAh Battery: Stay powered all day with the 6000mAh battery, offering up to 8 hours of mixed use for reading, gaming, or streaming. This Android 14 tablet can be fully charged via the USB Type-C port. It’s the perfect companion for work, study, or play!
+WiFi 6 &amp; BT 5.4 for Ultimate Connectivity: Experience lightning-fast internet speeds and stable connections with WiFi 6 and BT 5.4. This 10-inch tablet ensures smooth streaming, quick downloads, and seamless pairing with your favorite accessories. Whether you're browsing, gaming, or video calling, enjoy a lag-free experience.</t>
+  </si>
+  <si>
+    <t>imgamazon\710ofUNNVnL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>New Experience - The A30 Pad tablet is powered by the latest Android 15 OS, ensuring broader app compatibility, faster startup times, and improved responsiveness. The new system offers more customization, privacy, and security options, without the hassle of annoying ads.
+High Performance - Aiprotablet tablet is powered by the UNISOC T606 octa-core processor, featuring an ARM Cortex-A75 high-performance CPU and a Mali-G57 GPU, ensuring smooth and efficient operation of most apps and seamless multitasking.
+Ample Storage - The Android 15 tablet boasts 12GB LPDDR4x memory (4GB physical + 8GB virtual) and 64GB high-speed storage, expandable up to 2TB with a Micro SD card. You’ll have ample space for all your favorite media, including videos, photos, and more.
+Long-Lasting Battery - The 6000mAh battery lets you enjoy up to 8 hours of mixed reading, video watching, and web browsing. With the Type-C port and 18W PD fast charging, the tablet can be fully charged in just about 2 hours, saving you valuable waiting time.
+Large Touchscreen - The 10.1-inch tablet features a 1280x800 In-cell IPS display with a 16:10 aspect ratio, offering vivid colors and clear images for an enhanced viewing experience. The tailor-made case not only protects the tablet but also serves as a convenient stand.</t>
+  </si>
+  <si>
+    <t>imgamazon\71Z05qTBxRL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>MULTITASKING MASTER: The Lenovo Tab M11 combines robust performance with portability in a sleek design and easily switches between work or streaming
+POWER-PACKED PERFORMANCE: Streamline your day with the ability to work or study at home and on the go—the MediaTek Helio G88 Octa-Core processor delivers reliable mobile performance
+EXPERIENCE VIVID CLARITY: Immerse yourself in vibrant visuals—a 11" 1920x1200 WUXGA display brings your graphics and photos to life with stunning detail and precision
+DISCOVER SEAMLESS PRODUCTIVITY: Effortlessly juggle multiple applications and browser tabs without frustrating slowdowns, thanks to the generous 128GB SSD storage
+PLUG IN ON THE FLY: Easily connect your accessories and transfer files at lightning speeds with the USB-C port and 3.5 mm audio jack
+POWER UP FOR THE LONG HAUL: Harness your creativity wherever it strikes with up to 10 hours of uninterrupted battery life
+PREMIUM VIEWING AT ITS BEST: Enjoy a seamless viewing experience wherever you are thanks to the intelligent ambient light sensor
+CLEARLY CAPTURE EVERY MOMENT: Equipped with both front and rear cameras, the Tab M11 lets you effortlessly snap selfies, video chat with loved ones, and capture stunning photos
+TRAVEL WITH EASE: Designed with your mobile lifestyle in mind, this ultra-slim and lightweight tablet offers unparalleled portability
+ENABLING HUMAN-CENTERED OUTCOMES: At Lenovo, we strive to bring powerful methods of technology to our audience that will help create inclusive global change. We create each of our products while envisioning a world with smarter technology for all</t>
+  </si>
+  <si>
+    <t>imgamazon\71HCIiKPphL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>【2024 Fully Upgraded】2024 Newest 13.0 Android tablet, equipped with a powerful new Octa-Core processor, the maximum processing speed can reach 2.0GHz, and it has a significant effect improvement for multi-task management switching. Music, work, video, and games are sensitively controlled in the background and high-speed professional enjoyment.
+【Performance Leap】This Android 13 tablet has 128GB ROM+8GB RAM, 512GB additional expansion, which can store more games, movies, videos, music, and work software for you, and supports Netflix, Facebook, Tik Tok, Youtube, and other software, you can play more comfortably games, download and preview rich movies, and accommodate massive work files.
+【Specialized Design】This 2 in 1 tablet has built-in Bluetooth 5.0 and supports 5G/2.4G dual-band WIFI connection. It is suitable for more occasions, such as coffee shops, offices, and bedrooms. The strong receiving signal can keep you well connected all the time, allowing you to work happily, talk to family, and connect with friends anytime, anywhere.
+【Battery Life Upgrade】This Android tablet is equipped with an 8000mAh battery life upgrade, providing you with a longer user time, watching videos for up to 10 hours, playing games for up to 8 hours, and listening to music for more than 12 hours, bringing you more entertainment time and Internet time.
+【Ultra-Clear Design】This 10.1 inch tablet computer has an ultra-clear LCD screen, 1280x800 narrow-edge screen professional design, equipped with 13MP+8MP dual high-definition cameras, presenting you with richer picture display, clearer portrait capture, more delicate detail depiction, large screen Soft light curtain can reduce the visual pressure on your eyes and relieve fatigue.
+【Exquisite Tablet】This 2 in 1 tablet, equipped with a Bluetooth keyboard, mouse, and stylus, can be easily converted into a portable notebook and can be instantly converted into a work mode anywhere. This is the best tablet for colleagues, friends, family, and business people.
+【After Sales Service】MEIZE tablet computer professional team, focusing on customer service for more than ten years, adhering to the principle of customer first, with professional experience and excellent service, if you receive any problem products, please tell us anytime.</t>
+  </si>
+  <si>
+    <t>imgamazon\61yWWKPn4CL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>Android 14 Tablet: The C30 tablet is equipped with the latest Android 14 operating system, ensuring wider app compatibility, faster boot times and response times, optimized control over app permissions and giving you better control over your privacy and data.
+HIGH PERFORMANCE OCTA CORE PROCESSOR: The HNVHNV tablet is powered by the T606 octa core processor. Multitasking, high resolution video playback, or lightweight gaming is easy with this 10 inch tablet. With the pre-installed Play Store, you can download all your favorite apps!
+Plenty of storage: This Android 14 tablet has 10GB of RAM (4GB physical + 6GB virtual) and 64GB of internal memory, expandable to up to 1 TB with a micro SD card for storing your favorite photos, videos, and files. This gaming tablet is also GMS certified and Widevine L1 certified. You can access more HD content and streaming services on Hulu, and Amazon Prime Video.
+6000 mAh battery: The tablet has a 6000 mAh battery that supports up to 72 hours of standby time and 18 hours of video playback. With the USB Type C port and 18W PD fast charging, the tablet can be fully charged in about 2 hours, saving you valuable waiting time.
+10 inch FHD display: The tablet comes with a 10 inch HD IPS eye protecting display that reduces harmful blue light and reduces eye fatigue. 1280*800 pixels deliver brilliant colors and crisp images from all viewing angles. Equipped with 5MP+8MP dual cameras to optimize image processing. Face recognition, wireless screen casting, parental control, screen recording and other comprehensive functions make your tablet more convenient.</t>
+  </si>
+  <si>
+    <t>imgamazon\71ynGM76yjL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>EFFICIENT OFFICE COMPANION - This 14-inch Android tablet is powered by Android 14 and features a robust T616 octa-core processor with a clock speed of 2.0 GHz. The 14-inch screen provides a higher resolution, delivering clear and detailed visuals. This is particularly advantageous for design work or document processing, resulting in an enhanced viewing experience
+EFFICIENT HOME COMPANION - The 14-inch tablet computer is an excellent companion for both cooking and yoga. The tablet case can be folded in three different ways, providing various standing angles for taking Zoom calls, web browsing, drawing, and more. The triangular structure of the multi-fold folio ensures a stable position, whether in portrait or landscape orientation. This makes it ideal for following recipes while preparing meals or practicing yoga in any space
+UPGRADED ANDROID 14 TABLET - Callsky-Tab Ctab14 Android Tablet is equipped with the upgraded "Android 14" operating system. Android 14 Tablet enhances privacy and security while improving the overall user experience through personalized features, facial recognition for screen unlocking, and greater control over app data access. With a highly stable and secure network system, you can browse the web more smoothly and quickly using your Android 14 tablet
+10000mAh LONG LASTING BATTERY - The Ctab14 tablet is equipped with a powerful 10,000mAh battery, providing up to 14 hours of video playback. The Type-C port allows for easy charging, regardless of the orientation of the connector. Weighing just 996g, it is highly portable, making it convenient to carry whether you are working, studying, or on the go
+ULTIMATE TABLET ACCESSORIES &amp; GIFT CHOICE - To enhance the overall experience, we have prepared high-quality leather cases that not only provide protection but also add a touch of elegance. These cases are designed to fit perfectly, ensuring that your tablet looks stunning while remaining secure. Additionally, we offer a premium stylus that allows for precise and effortless navigation, drawing, and note-taking
+WIDEVINE L1 &amp; 14" SCREEN - This 14.1-inch tablet strikes a balance between portability and a satisfying visual experience. When paired with streaming services, the 14.1-inch display delivers an engaging viewing experience for movies, shows, and other media content. Our tablet features Widevine L1 support, which is the highest level of security offered by the Widevine system, enabling devices to stream content in HD (720p) or Full HD (1080p)
+2-YEAR MANUFACTURER WARRANTY - What truly sets us apart is our commitment to product quality. We offer an industry-leading 2-year extended warranty, providing you with peace of mind and assurance that your investment is protected. This extended warranty period reflects our confidence in the durability and reliability of our tablet, ensuring that you can enjoy it worry-free for years to come</t>
+  </si>
+  <si>
+    <t>imgamazon\71lfH8ihwSL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>[ Stable Android 14 System &amp; Octa-core CPU ] This 2025 NEWEST Android 14 tablet is equipped with a high-performance octa-core CPU, a stable Android 14 system with AI, and all functions have been strengthened to a new level. You will enjoy the smooth running of 12GB (6GB+6GB) RAM and 128GB ROM. Perfect for watching videos, learning, video chatting, and reading e-books easily .
+[ 11 Anti-blue Eyes Protection Screen ] This 11-inch tablet not only bigger screen, also features specific eyes protection HD 1280*800 fully-in-cell screen resolution, but the wide viewing angle also provides a more realistic viewing experience. With automatic brightness adjustment combined anti-blue light design for protecting your eyesight, you will be safer and more comfortable while using the tablet.
+[ Parental Control &amp; Face Unlock] Parental control helps children manage their time, balance learning and entertainment, and develop good online habits. Android 14 tablet also supports multi-window mode, eye protection mode, 3-finger screenshots and more to make the tablet experience even better. Face unlock functionality gives you convenient access to your wifi tablet.The dual camera allows you to take photos and make video calls.
+[ 8000mAh Large Battery + 18W Fast Charging] This rugged tablet built-in a 8000mAh large battery, you will freely enjoy reading or watching videos for 8-10hours on a full charge. No need to worry about the battery while you are traveling on the way . 18W USB-PD fast charging to reduce your charging time. (Note: 18W adapter sold separately,please use only 18W or 10W charge adapter not support 20W or 30W , and please have a charge more than 2 hours.）
+[ 128GB ROM Large Storge] 12GB RAM 128GB ROM storage, running stably. It easily expands to 1TB with a MicroSD card (sold separately) for storing photos, music, and videos without worrying about running out of space.
+[Compatible with Widevine L1] You can watch Amazon Prime Video, Disney+, Hulu, and more in high quality. *If the video distribution service imposes restrictions on compatible devices (eg: Netflix), image quality may be widevine L3.</t>
+  </si>
+  <si>
+    <t>imgamazon\71fyxOj0qFL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>𝟮𝟬𝟮𝟱 𝗡𝗲𝘄 𝗔𝗻𝗱𝗿𝗼𝗶𝗱 𝟭𝟰 𝗧𝗮𝗯𝗹𝗲𝘁: Powered by the latest Android 14 system, the tablet improves the performance and efficiency, gives users more control over their data and personal information, and enhances user information protection and accessibility features. Powered by an A523 Octa-Core processor with energy-efficient technology, this Android tablet achieve faster and more stable running and storage speeds. Tablet use more efficient, an excellent companion for life
+𝟭𝟭” 𝗙𝗛𝗗 𝗧𝗼𝘂𝗰𝗵𝘀𝗰𝗿𝗲𝗲𝗻 ＆ 𝗘𝘆𝗲𝘀 𝗣𝗿𝗼𝘁𝗲𝗰𝘁𝗶𝗼𝗻: The newly upgraded 11 inch tablet is equipped with a 1280x800 high-resolution touch screen, which has a larger screen, clearer and brighter images, and a wide viewing angle for a more realistic viewing experience. The tablet is equipped with automatic brightness adjustment and anti-blue light function to protect your eyesight, so that you can have a good time safer and more comfortable
+𝗔𝗱𝗲𝗾𝘂𝗮𝘁𝗲 𝗠𝗲𝗺𝗼𝗿𝘆 ＆ 𝗪𝗶𝗱𝗲𝘃𝗶𝗻𝗲𝗟𝟭: Experience unparalleled speed and storage with 16GB RAM (4GB Physical+ 12GB Virtual) and 128GB ROM. UGRIHACH tablet is GMS certificated, you can download any needed APPS from Play Store. Expand up to 1TB via TF card (not included) to keep all your favorite apps, photos, and files right at your fingertips. The Android tablets are WidevineL1 certified, you can stream HD content on platforms like Netflix and Amazon Prime Video, and enjoy crystal clear videos on the go
+𝗙𝗮𝘀𝘁 𝗖𝗼𝗻𝗻𝗲𝗰𝘁𝗶𝗼𝗻 ＆ 𝗦𝗺𝗼𝗼𝘁𝗵𝗲𝗿 𝗘𝘅𝗽𝗲𝗿𝗶𝗲𝗻𝗰𝗲: UGRIHACH Android tablet comes with WiFi 6, dual speakers and Bluetooth 5.3, and the tablet supports dual band WIFI for improved network stability and reduced network latency. This tablet comes with an 8 MP rear camera with focus and flash capabilities to ensure clear photos day and night. The 5 MP front-facing camera provides excellent clarity during video calls. The split-screen function makes multitasking a breeze. Dynamic Halo to set lighting effects for charging, music, games, and notifications
+𝗟𝗮𝗿𝗴𝗲 𝗖𝗮𝗽𝗮𝗰𝗶𝘁𝘆 𝗕𝗮𝘁𝘁𝗲𝗿𝘆 ＆ 𝗙𝗮𝘀𝘁 𝗖𝗵𝗮𝗿𝗴𝗲: The 6800mAh long-lasting battery paired with a ultra-high performance and low power consumption CPU, lets you enjoy extended playtime—whether for work, entertainment, or travel. UGRIHACH Android 14 tablet can be quickly charged through the Type-C connector (Headphone jack: Type-C)
+𝗜𝗱𝗲𝗮𝗹 𝗖𝗵𝗼𝗶𝗰𝗲 𝗙𝗼𝗿 𝗚𝗶𝗳𝘁 ＆ 𝗤𝘂𝗮𝗹𝗶𝘁𝘆 𝗚𝘂𝗮𝗿𝗮𝗻𝘁𝗲𝗲: With a thickness of only 1cm and a weight of only about 0.49 KG, this ultra-light tablet is designed for portability. This advanced and reliable UGRIHACH tablet is the perfect gift for your family or anyone who loves media and entertainment. In addition, we provide one year warranty for Android 14 tablet, if you have any quality problems, please contact us, we will assist you to solve the product problems</t>
+  </si>
+  <si>
+    <t>imgamazon\71fzL8zIrcL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>【High Performance】URAO Android tablet features the latest operating system Android 14 and an 2.0 GHz octa-core processor ensure of excellent performance, seamless multitasking, getting rid of annoying ads, emphasizing privacy and security by designing enhanced app permissions, providing you complete management control.
+【Massive Storage】Our tablet comes with 10GB (4+6GB) RAM 128GB ROM &amp; maximun 1TB TF card ( not included )expandable of a fast APP launch &amp; smooth gaming experience. URAO tablet come with pre-installed Google Play Store, you can easily download any needed Apps.
+【HD Eyes Protection】Equipped with high resolution 1280*800 IPS display, which shows a brightly colored wide-screen for a more realistic viewing experience with sharper and brighter images.Front&amp; rear cameras satisfy video calls, online learning, etc.
+【Large Capacity Battery with Fast Charge】Built-in large capacity and low consumption CPU enable our tablet to stand by for up to 3 days and allows you to enjoy up to 6 hours.URAO tablet dopts fast-charging technology which can be fully charged in 1.5 hour.
+【Wi-Fi 6+Bluetooth5.0】URAO android tablet 10 inch adopts the lastest sixth generation WiFi technology and the upgraded bluetooth 5.0. Dual band integrated chips make the 5g WiFi and 2.4g WiFi more stable and the lastest bluetooth 5.0 connection supports all your favorite accessories, highly increased the speed of data transfer, improved network capacity and reduced network delays.
+Note:The tablets have no GPS; tablet is based on Android system , cannot directly share accounts with IOS system.</t>
+  </si>
+  <si>
+    <t>imgamazon\61o0a4gGk8L._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>imgamazon\51nvMJJH7aL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>INNOVATIVE ART POWER: Turn your simple sketches into works of art instantly using Sketch to Image¹ with Galaxy AI.²
+SEARCHING MADE EASY: Quickly search for just about anything you see on your Tab — all without switching apps — using Circle to Search with Google.³
+MAKE A LONG STORY SHORT: Capture your lecture, meeting, or daily notes and let Note Assist⁴ with Galaxy AI² do the hard work of organizing and even summarizing them for you.
+NEXT-LEVEL NOTE TAKING: Get transcripts and summaries of recorded lectures and meetings, just like that.⁵
+PACKED WITH POWER: No matter what you take on or where you take your Galaxy Tab S10+, enjoy every experience with a powerful tablet processor.</t>
+  </si>
+  <si>
+    <t>imgamazon\71e4cAPBQDL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>JOY IN EVERY BEAT - Treat your senses to the Lenovo Tab Plus’s Octa JBL speakers and glittering 2K display. Redefine personal entertainment with its 175° kickstand and Bluetooth speaker mode for a perfect blend of visual and auditory delight. Plus, enjoy potection on the go with included folio case
+SOUNDS OF GOLD - Boost your vibes with Lenovo's industry-leading tablet sound system. The Octa JBL speakers enhanced by Dolby Atmos deliver booming power and crystal-clear highs and lows.
+DIVE INTO VISUAL LUXURY - Immerse yourself in a world where colors pop and details come to life on a 11.5” 2K screen. Enjoy your favorite shows and games in comfort with TÜV-certified eye care, safeguarding your vision day and night.
+NEXT-LEVEL ENTERTAINMENT - Elevate your gaming with the powerful MediaTek Helio G99 processor. Backed by the smooth 90Hz refresh rate and fast loading times, get ready for your new personal best.
+STANDBY MODE - Transform your tablet into a digital photo frame or beautiful clock when plugged in.
+YOUR PORTABLE DJ - Turn every spot into your personal party zone by utilizing the Bluetooth speakers. Enhance your audio landscape with precise volume controls for every app and playlist.
+DESIGNED FOR EXTRA CARE - Keep your tablet updated and secure with future OS upgrades and 4 years of security patches. Wrap your tablet in a responsibly crafted, all-around protection sleeve. It’s fashioned with DuPont Tyvek and PU leather to keep your tablet protected and chic wherever you go.
+FLEXABLE AND DURABLE - Experience 175° freedom with the integrated kickstand to enjoy your music and movies wherever life takes you.</t>
+  </si>
+  <si>
+    <t>imgamazon\71Yk4KqGb0L._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>【Android 14 Tablet, High Performance 8 Core CPU】2024 newest Android tablet 10 inch runs the latest OS, Android 14, and is also GMS certified, allowing users to download popular apps from the Google Play Store. Powered by the Unisoc T606 octa-core processor, this tablet ensures optimal performance for both work and multimedia, providing a seamless, energy-conscious tablet experience, suitable for gaming, high-definition video playback, and graphics-dense applications.
+[4G LTE calls and Dual 5G&amp;2.4G Wifi]: 2 in 1 Tablet, perfect combination of mobile phone and tablet. With the 4G phablet feature, Our tablet has Dual SIM capabilities that allow you to have two phone numbers in one device. You have both dual 5G&amp;2.4G Wi-Fi and 4G/3G/2G options for internet connectivity. Whenever Wi-Fi connection isn't available, you can rely on your data plan to connect to the internet. Notice: SIM CARD is NOT included.
+[14GB RAM+128GB ROM+2TB Storage]:The Android 14 Tablet is equipped with 14GB (8GB physical + 6GB virtual) RAM, and 128GB ROM with up to 2TB of TF card expansion support. Stores tons of movies, music, eBooks and more. The startup and response speed of the application is faster, allowing for smoother enjoyment of games, videos, or task processing.
+【10 inch FHD LCD In-cell Screen Tablet】ZONKO 10 inch large tablet use newest In-cell display, Not traditional screens, the in-cell technology integrates touch sensors directly into the display, which improves the sensitivity and accuracy of touch, reducing the thickness and weight, making movies more stunning, with 20% higher image clarity than normal displays. 16:10 screen ratio and wide color gamut provide a more realistic visual experience. The 10" ultra-thin and ultra-light gaming tablet enhance your experience, providing a more immersive journey while watching videos, playing games, or browsing the internet.
+【Multifunctional 2-in-1 Tablet】Android 14 tablet has rich tablet accessories, making it a perfect gift for friends and family. Accessories included: 1 x ZONKO Tablet, 1 x Tablet case, 1 x Bluetooth Keyboard, 1 x Wireless Mouse, 1 x Touch Pen, 1 x Sim/SD Card Pin, 1 x Screen Protector, 1 x OTG adapter, 1 x Type-C cable, 1 x charger , 1 x User Manual
+【8000mAhBattery+ 3.5mm Headphone Jack】This 128GB tablet with a 8000mAh battery, Type-C charging, built-in dual speakers and independent 3.5mm headphone jack will not interfere with each other when charging or listening to music, meeting your different needs.
+【Slim Metal Body+Dual 13MP Camera】The tablet's true of a full metal body, making the main body lighter and thinner. Convenient to carry around for work, study, or on the go. 13MP main camera with 8MP front-facing camera, ideal for video conferencing and calls and ensuring clear and It guarantees clear and professional visuals.</t>
+  </si>
+  <si>
+    <t>imgamazon\51LoFBO2UlL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>Charger Not Included. 8.7" (220.5mm), 1340 x 800 (WXGA+), TFT, 16M colors, Android 13, One UI 5.1
+64GB ROM, 4GB RAM, Mediatek Helio G99 (6nm), Octa-core, Mali-G57 MC2 GPU
+Rear Camera: 8MP, AF, Front Camera: 2MP, 5100 mAh battery, Bluetooth 5.3, USB Type-C 2.0
+No SIM Card Slot / Network - Wi-Fi Only.
+International Model without Domestic Warranty. The device is still covered by the Seller's Return Policy.</t>
+  </si>
+  <si>
+    <t>imgamazon\71AJ87m5ZDL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>【11-Inch In-Cell HD Display】: 11 Inch Tablet, Immerse yourself in a world of vibrant colors and stunning visuals on the expansive 11-inch in-cell HD screen. Whether you're streaming your favorite shows, browsing the web, or diving into the casual games, every detail comes to life, making your viewing experience better on this KADYBE Tablet.
+【2025 Latest Android 14 OS】: Unlock the full potential of your 2025 tablet with the cutting-edge Android 14 OS. Enjoy a seamless and intuitive user experience, complete with the latest features and enhancements that make multitasking a breeze. Android 14 tablets better protects your privacy and is able to work with a variety of apps you want to download.
+【Impressive 16+128+1TB Memory】: Say goodbye to storage worries! This tablet boasts a powerful combination of 16（8+8Virtual）GB RAM and 128GB internal storage, expandable up to a whopping 1TB. Store all your favorite apps, photos, videos, and documents without compromise, ensuring you have everything you need at your fingertips.
+【Large Battery+21MP Camera】: Android tablet with a large 8000mAh battery for your busy life, so you can experience uninterrupted use. Capture life's moments in stunning detail with the 13+8MP rear+front camera, perfect for on-the-go use. Share your adventures with friends and family using this KADYBE tablet!
+【4G SIM Card and Wi-Fi Support】: Stay connected at anywhere and anytime on this Android 14 tablet 11 Inch. With dual connectivity options for 5+2.4Ghz WiFi and 4G SIM card support, you can enjoy fast and reliable internet access wherever you are. Whether you're working remotely or streaming content, you’ll never miss a beat.
+【Powerful Octa-Core processor】: This 2 in 1 Android 14 Tablet is equipped with a powerful MTK8786 processor with up to 2.0Ghz. Whether it's multitasking, gaming or HD video playback, this tablet can handle it with ease, ensuring you enjoy fast response and efficient operation in any situation.
+【Full Package with 1 Year Support】: 2 in 1 tablet with keyboard provides a full package, which includes a bluetooth keyboard, responsive wireless mouse, a stylish protective case, 2pcs screen protector and usb-c cable and charger. Enjoy peace of mind with our dedicated lifetime customer support and a 365days manufacturer warranty.</t>
+  </si>
+  <si>
+    <t>imgamazon\71fkPYZOKgL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>Windows 11 Professional for Advanced Productivity: Experience seamless multitasking and enhanced flexibility with Windows 11 Pro on the Fusion5 232 Pro N5. This professional-grade windows tablet adapts effortlessly to your work and creative pursuits, offering an intuitive interface and powerful performance for modern users.
+Powerhouse Performance: The Fusion5 232 Pro N5 redefines tablet pc computing with its Intel Alder Lake 13th Gen N100 CPU, delivering speeds up to 3.4GHz. Paired with 8GB LPDDR5 RAM and a 256GB M.2 SSD, this windows 11 tablet ensures lightning-fast responsiveness, smooth multitasking, and amazingly quick boot times for professionals and everyday users alike.
+Stunning Display for Digital Vibrance: Immerse yourself in a breathtaking viewing experience with the Fusion5's 10.1" 1920*1200 FHD IPS display. This tablet windows 11 delivers vibrant colors and sharp clarity, complemented by a durable G+G 2.5D capacitive touchscreen for precise and responsive interaction.
+Versatile Connectivity Options: Stay connected with ease using the tablet with USB port, USB Type-C, and Micro HDMI for swift data transfers and external display connections. The computer tablet windows also supports a Micro SD slot (up to 512GB) and an optional docking keyboard (sold separately), transforming it into a highly efficient tablet computer.
+Why Choose Fusion5? This ultra-slim and stylish tablet windows checks all the boxes for usability, performance, and design. Backed by a 12-month full USA warranty and support from our dedicated service center, it ensures a worry-free ownership experience. Fusion5 computer tablets deliver the perfect combination of power, style, and reliability.</t>
+  </si>
+  <si>
+    <t>imgamazon\71SIng0h1TL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>UPGRADED 4K DIGITAL CAMERA WITH FLASH &amp; SELF-VLOGGING : This digital camera uses the latest &amp; advanced CMOS chip, helping you take &amp; record the most exciting moments in 48 MP quality images &amp; 4K Ultra HD quality videos, there is also a built-in flash to help you take high quality pictures even in low light &amp; dark settings, ideal for indoors outdoors. This 4k vlogging camera has a 3'' 180°Flip LCD Screen, you can see what you are recording or the picture framing while doing self blogging.
+LATEST AUTOFOCUS 4K CAMERAS for PHOTOGRAPHY with FLASH &amp;16X DIGITAL ZOOM : This digital camera for Photography supports Auto-Focus, it is faster, clearer and more accurate to capture the subject you want, and almost unaffected even in strong light environment. This 4K vlogging camera supports 16x digital zoom, allowing you to easily zoom in or out by pressing the W/T button during video recording and for taking still images.
+4K CAMERA with BATTERY CHARGING STAND &amp; HOT SHOE MOUNT : Equipped with 2 batteries and a charging stand, No need to charge the battery with a camera, easier to charge a spare battery by charging stand , the charging stand is carried anywhere in your handbags or pocket. Take this camera along on trips or for any traveling activity/camping/going hiking or just about any sport imaginable. Equipped with hot shoe mount, can be connected to Flash Light , soft light, and MIC.
+WEBCAM FUNCTION &amp; HDMI OUTPUT : Using video mode with the built-in microphone, you'll be able to record quality videos for all your vlogging and YouTube needs. This compact camera can be used as a Webcam, please insert the USB cable and switch the camera to "Webcam" mode, ideal for video calling, live streaming, blogging, vlogging, online teaching, etc. This 4k digital camera also has HDMI output for playing back the videos on TV.
+MULTIFUNCTIONAL PORTABLE DIGITAL CAMERA 4K : This compact camera is equipped with many features such as anti-shake, fause function, continuous shooting, time-lapse shooting, slow motion, motion detection, self-timer, time stamp ON/OFF, making this the camera for all indoors/outdoors situations. Our dedicated and experienced 24/7 customer support team is available for all after purchase troubleshooting, questions and technical help.</t>
+  </si>
+  <si>
+    <t>imgamazon\61JavBEclHL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>SHOOT DECENT IMAGES WITH EASE - The digital camera captures high-clarity FHD 1080P videos and 44MP photos with the newest CMOS metering system, no need for complicated manual settings while delivering natural color images automatically. One second to press the shutter, it's easy for starters and kids.
+PORTABLE FOR TRAVEL &amp; NICE BATTERY LIFE - The kids camera is a perfect everyday and take everywhere camera with it's petite body, durable, lightweight and small enough for your pocket. With two large capacity batteries, charging several times can last for one month. Plus, the automatic turn-off setting saves more energy in vacation trips and camping.
+VERY EASY TO USE - Conducted with ergonomic design, from easy to access buttons to simple functions menu, user-friendly interfaces down to the large LCD display, a 5-13 years kid can easily figure out. Just install the SD card, battery, two seconds to turn it on, and freely capture all fun memories with friends, family.
+ENCOURAGE CREATIVE - If you are tired of its automatic results, the point and shoot camera allows you to customize pictures. 16X zoom is great for photographing objects in the distance. 20 pcs creative filter effects to take Vintage photos, Black/White photos..., Anti shake, webcam, face and smile detection, continuous shooting, self-timer, waiting for you to explore them.
+SUPERIOR SUPPORT FOR THIS GIFT - Backed by a one year hassle-free promise- refund and replacement. Digital camera, SD card, lanyard, storage bag, batteries, adapter, cable, exquisite box..., contains everything you need. It is a perfect gift for boys, girls, teens on birthdays, Christmas or any important events, a first real camera for kids who love to take videos and pictures.</t>
+  </si>
+  <si>
+    <t>imgamazon\81swjZCbdiL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>16 Megapixel CMOS Sensor
+5X Optical Zoom - 28mm Wide Angle Lens
+1080P Full HD Video - Vlogging Camera
+SD Card Compatibility: At least Class 10, no more than 512GB (SD, SDHC, SDXC)
+2.7" LCD Screen - Rechargeable Li-Ion Battery</t>
+  </si>
+  <si>
+    <t>imgamazon\71iABxYS-eL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>4x Optical Zoom - 27mm Wide Angle Lens
+16MP CMOS Sensor
+1080p Full HD Video - Vlogging Camera
+SD Card Compatibility: At least Class 10, no larger than 512GB (SD, SDHC, SDXC)
+2.7" LCD</t>
+  </si>
+  <si>
+    <t>imgamazon\71Ed3wdBvhL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>【4K UHD Video &amp; 48MP Photo Capture, Record Every Special Moment】 This compact digital camera features the latest CMOS sensor system, supporting 4K video recording and 48MP high-resolution photos. Whether you're exploring the beauty of nature or capturing the joy of a family gathering, this camera ensures you can clearly document every important moment in stunning detail.
+【16X Digital Zoom &amp; Versatile Shooting Modes】 Want to capture distant landscapes or zoom in on wildlife? With 16X digital zoom, this camera allows you to bring distant subjects into focus with ease. The built-in image stabilization ensures your photos are steady and sharp. Features like smile capture, continuous shooting, and self-timer make it the perfect choice for documenting family gatherings, friend parties, and other joyful moments.
+【Smart Autofocus, Effortlessly Capture Any Scene】 Whether you're at a friend's birthday party or a child’s sports event, the camera's autofocus system ensures you can easily capture every important moment. Simply press the shutter button for precise focus, and then press again to snap the photo, guaranteeing each shot is clear and crisp.
+【Webcam Function &amp; Record While Charging】 Video calls for work, school, or family gatherings have never been easier. Switch the digital camera to Webcam mode after connecting to your computer, and enjoy smooth video calls or live-stream your experiences with friends and family. Plus, with the ability to record while charging, you don’t need to worry about running out of battery during long recording sessions.
+【Compact &amp; Travel-Friendly with Complete Accessories】This protable small digital camera is perfect for travel or everyday use, easily fitting into your bag or pocket. It comes with a 32GB SD card, 2 batteries, and a Type-C charging cable, making it ready to use anytime. The 2.8-inch IPS screen provides an intuitive interface, so you can quickly view, edit, and share your photos. Whether as a gift for friends and family or a companion to document your own life, this camera is the ideal choice.</t>
+  </si>
+  <si>
+    <t>imgamazon\81Q5HtrSzuL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>[Rugged Digital Camera] This compact digital camera, small enough to easily slip into your pocket, boasts a sturdy yet sleek design. It's engineered to shoot effortlessly underwater up to 33 feet, resist dust, and even withstand falls from heights of up to 4 feet unscathed. With its superior adaptability to harsh environments compared to your smartphone, it's the ideal choice for adventurers and outdoor enthusiasts. Whether you're diving deep or soaring high, this camera is a powerful tool for capturing exciting moments.
+[8KUHD Recording and 70MP Photo] Capture the world in stunning 8K ultra-high definition, offering a more vivid and intricate video experience compared to traditional 4K cameras. With a 70MP photo capability, details come to life with remarkable clarity. It effortlessly captures the majestic landscapes of your travels, meets the precision required for detailed work projects and real estate photography. Whether you're hiking, camping, at the beach, or snorkeling, it's the perfect companion. Even kids can easily snap high-quality photos, preserving every unforgettable moment.
+[Autofocus &amp; Macro Capability] This 8K autofocus camera elevates clarity to new heights. Its macro shooting feature allows you to get as close as 1.97" to your subject. When the autofocus frame shifts from red to green, it signals that focus is locked. Fully press the shutter button at this point, and you can capture the intricate details of even the tiniest creatures in crystal-clear precision. From the texture of corals to the scales of a small fish, everything unfolds in stunning clarity.
+[2500mAh built-in Battery &amp; SOS Light] Our underwater camera comes equipped with a large-capacity 2500mAh battery, ensuring up to 2.5 hours of continuous video recording. Capture precious moments to your heart's content without worrying about battery life. In times of danger, the built-in SOS flashlight can quickly draw attention, adding an extra layer of safety. Moreover, the included 32GB storage card can store up to 8,000 photos, ensuring no moment of your adventure goes uncaptured.
+[User-friendly Design] Our waterproof camera, now upgraded in size, offers an enhanced viewing and shooting experience. Standing out from the common 16:9 screen ratio, this camera features a 2.88-inch high-definition front screen and a 1.44-inch high-definition rear screen, adopting a 4:3 aspect ratio. This provides a more comprehensive viewpoint, optimizing framing and composition. Say goodbye to cramped screens and enjoy a broader view that brings your photography to life.</t>
+  </si>
+  <si>
+    <t>imgamazon\819UX5S0I2L._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>【5K UHD &amp; 75MP Video Camera】This digital camera captures stunning 75-megapixel images and shoots vibrant 5K Ultra HD video with rich colors and crisp details. Take your photography to the next level with a variety of built-in filters for a uniquely creative experience.
+【Autofocus &amp; 18X Digital Zoom Camera】This photography camera boasts a robust 18x digital zoom, allowing you to capture distant objects with ease. The autofocus feature ensures your shots are always sharp, so you can effortlessly capture perfect moments. The vlogging camera also features a 3.0-inch IPS 180° flip HD screen, making it perfect for snapping selfies from any angle.
+【Wireless WIFI &amp; Webcam/Vlogging Function】The upgraded camera for YouTube features a built-in wireless Wi-Fi function, allowing you to instantly share videos and photos online via your cell phone. This vlog camera can also be used as a webcam for live streaming, video calls, and blogging, making it easy to stream or make video calls on YouTube, Facebook, Twitter, or other social media platforms.
+【Rechargeable Battery &amp; 32GB SD Card】Equipped with two high-capacity batteries and a 32GB SD card, this compact camera ensures you never miss a moment. The built-in flash allows you to capture those wonderful memories even in low-light environments. Plus, the camera is tripod-compatible, making it perfect for stabilizing long shots during vacations and camping trips.
+【Point and Shoot Camera Easy to Operate】Designed for effortless use, this 5K digital camera is perfect for beginners, kids, teens, students, and seniors alike. Intuitive buttons and user-friendly menus make capturing moments as easy as pressing a button.</t>
+  </si>
+  <si>
+    <t>imgamazon\71t0fxzgqVL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>【4K 60FPS Action Camera &amp; 8X Zoom】 The 4K 60fps video and 64MP photos provide crisp and vibrant footage that captured the fast-paced fun and stunning scenery. Equipped with the 8x digital zoom, the action camera allows you to get closer to your subject. Perfect for hiking, climbing, biking, skateboarding, snowboarding, skiing, skydiving, hunting, and other outdoor adventures.
+【Dual Screen &amp; Compact Design】The dual-screen design, featuring both front 1.5” and rear 2” IPS, is a game-changer for framing shots. The rear screen is touch screen that is intuitive and easy to adjust settings and capture great shots. The sports camera's compact size and durability design make it perfect for capturing action-packed moments and handle a bit of extreme sports.
+【Without the Waterproof Case up to 65 Feet 】 The IP68 waterproof design of underwater camera can withstand depths of up to 65 feet (20 meters) without the waterproof case. Perfect for water sports like swimming, surfing, kayaking, snorkeling, and diving. While the two rechargeable 1350mAh batteries ensure extended recording time, making it a reliable companion on a recent road trip.
+【Built-in WiFi &amp; Wirless Sharing】 The sports camera comes with the Live DV APP and 2.4G WiFi connection, which makes it easy to get photos and videos off your camera directly. Notes: It needs to download the footage to your phone by APP firstly before transferring and sharing footage. The EIS (Electronic Image Stabilization) helps smooth out videos, reducing shake, which is great for high-intensity activities.
+【Multitude of Features &amp; Reliable Customer Support】 The action camera also offers upside down mode, loop recording, time-lapse, slow-motion, self-timer, screen saver and burst photo. The sports camera comes with a bunch of mounting accessories, making it versatile for various activities. Plus, the impressive replacement and lifetime customer support are noteworthy.</t>
+  </si>
+  <si>
+    <t>imgamazon\71NMGgXWa2L._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>[48 MP &amp; FHD 4K Digital Camera for Photography]- YOODEE 2025 compact digital camera support premium 48MP photos and 4K HD video recording. Advanced CMOS technology ensures precise detail,capture vivid picture for preserving your every important moment.The 16x digital zoom point and shoot camera with anti-shake feature is ideal for beginners to capture distant scenery.
+[Auto Focus Dual Cameras with 2.8" IPS Screen ]- Innovative dual camera design! Switch to the front camera for easy selfies with just one click, and the rear camera easily unlocking various shooting skills. 2.8" IPS screen 4k digital camera supports a powerful focusing function to ensure precise focus of the front and rear lenses, allowing you to easily capture clear photo. Our 4k autofocus digital cameras perfect as a birthday or graduate gift.
+[2 Batteries &amp; Flash Light &amp; Anti-Shake]-The travel digital camera is smaller &amp; lighter than a mobile phone and can easily fit into your pocket. 4k camera is equipped with two 700mAh large-capacity batteries allowing you to replace the batteries at any time to keep continue shooting. In addition, the 4k vlog camera used for photography and recording life has been upgraded with flash and anti-shake design, which can take clear photos and videos even in dim environments.
+[Webcam &amp; Pause Function]-This vlogging camera supports video mode, built-in microphone and anti-shake function, connect to computer via USB cable and used as webcam for video calls and live streaming, so you can share your wonderful moments to social media. YouTube Camera for vlogging has an excellent pause feature that allows you to pause while recording your video. Blog portable camera perfect for recording happy moments with friends, family members, indoors/outdoors
+[Multifunction &amp;Easy To Use]-This 4k video camera comes with a 32G TF card supports multifunction, the camera is a webcam, face detection, smile capture, continuous shooting, selfie, beauty function, shutter balance, auto close etc.This small camera is the best gift for kids,teenagers,beginners and the elderly. The camera digital offer after-sales protection,If you have any problems or concerns, please feel free to contact us,we will give you a satisfied solution within 24 hours.</t>
+  </si>
+  <si>
+    <t>imgamazon\71KO7VHuWuL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>Crystal Clear Imaging: Capture stunning visuals with a 56MP sensor that ensures every detail is preserved, providing images in unparalleled clarity. Whether you're snapping breathtaking landscapes or intimate portraits, the camera's high resolution ensures vivid and lifelike pictures.
+Versatile Video Capabilities: Seamlessly transition from photography to video graphy with 4K Ultra HD and 1080p video recording capabilities. Preserve your memories in cinematic quality, and share your adventures with friends and family in stunning high definition.
+Zoom In, Stand Out: Elevate your photography game with the 20X digital zoom feature, allowing you to get up close and personal with your subjects without compromising image quality. From distant landscapes to wildlife, this camera ensures that no detail goes unnoticed.
+On-the-Go Convenience: Designed for travel enthusiasts, this portable digital camera is compact and lightweight, making it the perfect companion for your adventures. Slip it into your pocket or bag, and capture moments wherever you go. It's not just a camera; it's a travel essential.
+Multifunctional Marvel: Beyond its primary role as a powerful camera, this device doubles as a webcam, enhancing your virtual meetings with crisp and clear video. Its multifunctionality makes it a versatile gadget for both professional and personal use, adapting to your diverse needs effortlessly.</t>
+  </si>
+  <si>
+    <t>imgamazon\61VsJsjJ-kL._AC_SL1200_.jpg</t>
+  </si>
+  <si>
+    <t>Waterproof to 15m (49') - 2m (6') Shockproof Rating - Dustproof
+WiFi Connectivity - 1080P Full HD Video - Vlogging Camera
+16 MegaPixel BSI CMOS Sensor - 4X Optical Zoom - Digital Image Stabilization
+Rechargeable Li-Ion Battery - 2.7" LCD Screen
+SD Card Compatibility: At least Class 4, no larger than 32GB (microSD, microSDHC) - MMC Card not supported</t>
+  </si>
+  <si>
+    <t>imgamazon\71R1OY2TTOL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>HIGH-PERFORMANCE CMOS SENSOR: ROQIOO digital camera uses the latest CMOS metering system to easily capture high-quality images, capture high-definition FHD 1080P videos and 48MP photos, and our company has optimized the operation interface according to a large number of products on the market, so that beginner children can master the use more easily and quickly
+INNOVATIVE AUTOFOCUS &amp; 16X DIGITAL ZOOM: This compact digital camera has an innovative autofocus function, you can half-press the shutter button when taking pictures to automatically focus, so as to get the clearest and most vivid photos. You can also use the W/T button to adjust the 16x digital zoom to shoot scenery from a distance, clearly capturing all the moments you want.
+MINI &amp; LONG BATTERY LIFE: This camera for kids is compact and easy to carry. Children can easily put it in a backpack or pocket to capture the beautiful moments in life at any time. Equipped with a high-efficiency battery to ensure long-term shooting, so that children can enjoy the fun of taking pictures whether in outdoor adventures or family gatherings, without frequent charging, and enjoy recording every wonderful moment.
+EXQUISITE ACCESSORIES &amp; PERFECT EXPERIENCE: Each children's camera is equipped with simple and stylish packaging, which is not only suitable as a gift, but also shows high-quality design. At the same time, we have prepared a portable storage bag for the camera, which is convenient for children to store and carry when going out, ensuring the safety of the camera. In addition, the included data cable is convenient for quick charging, and the camera lanyard helps children keep stable when shooting to avoid falling. Make every shooting smoother and more enjoyable!
+EXCELLENT FUNCTIONS &amp; EASY SHOOTING: This compact camera not only has anti-shake technology to make children more stable when shooting and avoid blurry images, but also acts as a webcam. Not only that, it also has a variety of fun special effects built in, such as black and white photos and smile detection, so that children can use their creativity when shooting and take unique works</t>
+  </si>
+  <si>
+    <t>imgamazon\71upuaX0zDL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>【𝟒𝐊 𝐔𝐇𝐃 𝐕𝐢𝐝𝐞𝐨 &amp; 𝟔𝟒𝐌𝐏 𝐈𝐦𝐚𝐠𝐞𝐬 𝐃𝐢𝐠𝐢𝐭𝐚𝐥 𝐂𝐚𝐦𝐞𝐫𝐚】The CAMWORLD Digital Camera 4K provides 4K UHD videos and 64MP photos, ensuring the images captured are clearer and more beautiful, making you fall in love with photography.
+【𝐃𝐮𝐚𝐥 𝐒𝐜𝐫𝐞𝐞𝐧 𝐃𝐞𝐬𝐢𝐠𝐧 &amp; 𝐎𝐧𝐞-𝐭𝐨𝐮𝐜𝐡 𝐀𝐮𝐭𝐨𝐟𝐨𝐜𝐮𝐬】This 4k digital camera is equipped with a 1.4-inch front HD display, which can easily achieve perfect selfies (press the "OK" button for 3 seconds to switch to the front screen selfie mode), and a 2.8-inch rear display to take clearer pictures. This vlog camera can meet all your shooting needs.And the camera is equipped with a One-touch Autofocus function, which can easily focus and take clearer pictures by half-pressing the shutter button.
+【𝟏𝟖𝐗 𝐃𝐢𝐠𝐢𝐭𝐚𝐥 𝐙𝐨𝐨𝐦 &amp; 𝐅𝐢𝐥𝐥 𝐋𝐢𝐠𝐡𝐭 𝐅𝐮𝐧𝐜𝐭𝐢𝐨𝐧】This digital cameras has 18x digital zoom, which can easily capture every detail, whether close or far, ensuring that your footage is always clear and vivid. The travel camera is also equipped with a fill light to supplement the light source. Allowing you to take high-definition photos and videos in low-light conditions or dark conditions.
+【𝐖𝐞𝐛𝐜𝐚𝐦 𝐟𝐨𝐫 𝐋𝐢𝐯𝐞 𝐒𝐭𝐫𝐞𝐚𝐦𝐢𝐧𝐠】This versatile vlogging camera doubles as a webcam and supports tripod mounting (not included) for video calls, live broadcasts, or online teaching on TikTok, YouTube, and Facebook. Easily transfer photos/videos to your computer or smartphone to share good times with your loved ones.
+【𝐂𝐨𝐦𝐩𝐚𝐜𝐭 𝐃𝐞𝐬𝐢𝐠𝐧 𝐚𝐧𝐝 𝐋𝐢𝐠𝐡𝐭𝐰𝐞𝐢𝐠𝐡𝐭 𝐂𝐚𝐦𝐞𝐫𝐚】This compact and beautifully designed travel camera can be easily put into your pocket or bag, making it very convenient to carry with you, ready to capture any moment of inspiration. It also comes with all the accessories you need: rechargeable battery and USB Type-C data cable, 32G SD card and battery, lanyard and handbag, and cleaning cloth.
+【𝐏𝐞𝐫𝐟𝐞𝐜𝐭 𝐠𝐢𝐟𝐭 𝐰𝐢𝐭𝐡 𝐠𝐫𝐞𝐚𝐭 𝐦𝐞𝐚𝐧𝐢𝐧𝐠】This samll camera digital is a meaningful perfect gift for different ages, different occasions and different festivals. It is suitable for birthdays or holiday gifts for children, teenagers, the elderly, family, friends, beginners, and record the beautiful moments of life.</t>
+  </si>
+  <si>
+    <t>imgamazon\71n7+F1ocIL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>Ultra HD: The digital camera uses SONY's CMOS pixel sensor and can support shooting up to 80MP photos and UHD 5K videos.
+18X Zoom: The kids camera supports 18X zoom and auto focus, which is easy to use for beginners.
+Video recording: This small camera supports slow-motion video and time-lapse video, making it easy to record wonderful moments.
+Photography: Cameras for photography supports continuous shooting, automatic shooting, timed shooting and other functions.
+Adjustable parameters: Camera for kids supports 7 exposure levels, 8 colors and 5 filter adjustments, allowing children to learn more photography skills during use.
+Packing list: The package includes 1 point and shoot digital cameras, 2 batteries, 1 64GB TF Card, 1 USB-C cable, 1 lanyard and an instruction manual.</t>
+  </si>
+  <si>
+    <t>imgamazon\61BKYlNqH6L._AC_SL1000_.jpg</t>
+  </si>
+  <si>
+    <t>24.1 Megapixel CMOS (APS-C) sensor with is 100–6400 (H: 12800)
+Built-in Wi-Fi and NFC technology
+9-Point AF system and AI Servo AF
+Optical Viewfinder with approx 95% viewing coverage
+Use the EOS Utility Webcam Beta Software (Mac and Windows) to turn your compatible Canon camera into a high-quality webcam. Compatible Lenses- Canon EF Lenses (including EF-S lenses, excluding EF-M lenses)</t>
+  </si>
+  <si>
+    <t>imgamazon\81C9A0E+8TL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>40X Optical Zoom - 24mm Wide Angle Lens
+20 Megapixel CMOS Sensor
+1080P Full HD Video - Vlogging Camera
+SD Card Compatibility: At least Class 10, no larger than 512GB (SD, SDHC, SDXC)
+3" LCD Screen - Optical Image Stabilization (OIS) - AA Batteries</t>
+  </si>
+  <si>
+    <t>imgamazon\814TdrBdVQL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>【2024 Upgraded Digltal Camera】This camera uses the latest &amp; advanced CMOS chip, 56 MP quality images &amp; FHD 1080P quality videos,there is also a built-in fill light to help you take high quality pictures even in low light&amp;dark settings.This camera is an ideal thing for kids, adults, and everyone. Designed for kids, teens, and beginners, this point-and-shoot digital camera requires no intricate setup. Ideal for nurturing kids' interest in photography and crafting delightful moments with family and friends.
+【Small but Powerful】This kids camera supports 16x digital zoom.Plus, this small camera is also equipped with many features such as anti-shake, face recognition, smile detection, continuous shooting, self-timer, time stamp ON/OFF, making this the perfect camera for all indoors/outdoors situations. And it’s easy to operate, just press the shutter button fully to take pictures.
+【Very Easy To Use 】Conducted with ergonomic design, from easy to access buttons to simple functions menu, user-friendly interfaces down to the large LCD display, a 5-13 years kid can easily figure out. You can effortlessly transfer your images from the digital camera to your computer, just use the included USB data cable to connect the camera to the computer. We also included a 32GB TF card to make sure you have enough storage space.
+【Portable For Travel &amp; Nice Battery Life】The kids camera is a perfect everyday and take everywhere camera with it's petite body, durable, lightweight and small enough for your pocket. With two large capacity batteries, charging several times can last for one month. Plus, the automatic turn-off setting saves more energy in vacation trips and camping.
+【Warranty &amp; Package List 】We provide a one-year satisfaction warranty, along with a no-hassle replacement policy, any problem or question with the camera, please contact us for help.The package included 2x Batteries,1x 32GB TF card,1x USB cable, 1x kids digital camera,1x Lanyard and Bag.</t>
+  </si>
+  <si>
+    <t>imgamazon\81aVXv3w2dL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>25X Optical Zoom - 24mm Wide Angle Lens
+16 Megapixel CMOS Sensor
+1080P Full HD Video - Vlogging Camera
+3" LCD
+3" LCD Screen - Optical Image Stabilization (OIS) - AA Batteries</t>
+  </si>
+  <si>
+    <t>imgamazon\716gp4ChszL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>Ultra-wide 20mm* lens gets it all in the frame, even at arm’s length
+Large 1” sensor and F2 lens, for low-light and defocusing backgrounds
+Stay focused with Eye-AF* and autofocus tracking technology
+Side-articulating touchscreen LCD for easy to compose selfie shots
+Clear Voice with directional 3-Capsule mic and wind screen accessory4</t>
+  </si>
+  <si>
+    <t>imgamazon\81DiHPULy2L._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>Panoramas in Extraordinary Detail: 20mm wide-angle lens creates breathtaking landscapes, with a powerful 60x zoom (35mm equivalent: 20-1200mm) to capture the big picture as well as fine details
+An Always-Clear View, Even in Bright Sunlight: 2,360K-dot. Large LVF 0.74x (35mm camera equivalent) ensures you'll see your screen without glare
+Amazing Video Quality for Fast-Paced Action: 4K Video Mode records up to 4x resolution of Full HD; for incredible flexibility; 4K Photo feature lets you extract the perfect 8-megapixel photo out of 4K video and save it
+Shoot Now, Focus Later: Post Focus feature gives you the power to touch the area you'd like to be in focus, even after the shot has been taken
+No More Blur, Even at 60x Zoom: The POWER O.I.S. (Optical Image Stabilizer) effectively suppresses hand-shake vibration at the tele-end</t>
+  </si>
+  <si>
+    <t>imgamazon\71ni4J+T6JL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>Capture Stunning 4K &amp; 48MP Photos: Preserve your precious memories in breathtaking 4K Ultra HD video and 48MP high-resolution images with this digital camera.
+16X Digital Zoom &amp; Autofocus: Get closer to the action with 16X digital zoom and capture sharp, detailed photos with autofocus, even from a distance. Pressing the shutter release button halfway when taking a photo with this 4K digital camera and again when the focus frame changes from yellow to green ensures that every shot is in sharp focus.
+3.0" IPS 180° Flip Screen for Perfect Selfies &amp; Vlogging: The 3.0-inch IPS flip screen rotates 180°, making it easy to frame yourself for stunning selfies and vlogs. This portable compact digital camera is perfect for travel, vacations, and everyday use, fitting easily in your pocket or bag.
+Never Miss a Moment with 2 Rechargeable Batteries &amp; 32GB card: This 4K vlogging camera comes with 2 rechargeable batteries and a high-quality 32GB card, you can shoot all day without worrying about running out of power.
+Unleash Your Creativity with Advanced Features: Explore your creativity with 4K point and shoot camera's features like date stamp, video pause &amp; play, time-lapse, slow motion, fill light, anti-shake, 3 continuous shooting, smile &amp; face detection, beauty face, selfie, and various filters.</t>
+  </si>
+  <si>
+    <t>imgamazon\711X0g9zd5L._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>4 K &amp; 64 MP cameras for photography: Multiple video and photo sizes are up to you - video resolution：4 K /2.7 K /1080 P/720 P/360 P; photo pixel:64 M/56 M/48 M/30 M/24 M/20 M/12 M/8 M
+Doubles as A Webcam &amp; Pause Function:Connect to PC and work as webcam to video calling. The camera have an excellent PAUSE FUNCTION which allows you to continue recording in the same File without restarting a new one
+WiFi &amp; HDMI Output Function: Saneen WiFi camera makes you can share the photos and videos online with mobile phones instantly.This camcorder supports TV output and can be connected to TV to share your video with family
+4.0" Touch Screen &amp; Dual-Lens camera: This camera supports 4.0-inch touch screen. Equipped with dual lens,easy switching to front camera, you can see what you are recording or the picture framing while doing self blogging
+What You Get: Bundle Items Include: Camera x 1; 3000mAH Lithium Battery x1; USB cable x1; User Manual x1；32GB card x1, Lanyard x1,Lens Hood x1,Camera bag x1. We provide 12 months warranty, 30 days no reason to return
+There are very important points about external microphones that need attention: 1. The external microphone needs its own power supply, the camera cannot power the microphone
+There are very important points about external microphones that need attention: 2. The external microphone must be a dual-channel microphone with a 3.5mm connector
+Please pay attention：This is a regular camera suitable for beginners, teenagers, and non professionals with low-level needs. It is not suitable for professionals who have high requirements for photography, such as requiring the same image quality and video quality as professional cameras</t>
+  </si>
+  <si>
+    <t>imgamazon\7127mWGA51L._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>52x Optical Zoom - 24mm Wide Angle Lens
+16 MegaPixel CMOS Sensor - 6 frames per second Burst Shooting - 1080P Full HD Video - Vlogging Camera
+Wi-Fi Connection with the ability to Wirelessly Control with iOS or Android Devices
+SD Card Compatibility: At least Class 4, no larger than 32GB (SD, SDHC)
+3" LCD Screen - Rechargeable Li-Ion Battery</t>
+  </si>
+  <si>
+    <t>imgamazon\61G+brHcWJL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>imgamazon\71OG4+0m4GL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>5K Digital Camera with Greeting Card：Ultra HD 5K video shooting brings clearer details and true colors, 80MP ultra-high pixel photography performance can capture every fine texture and rich layers (L*W*H: 4.33*0.96*2.66 Inches,Weight: 0.7lbs)
+2.8'' Scratch-Resistant Tempered Screen：The pink camera equipped with a durable, scratch-resistant tempered screen that resists daily wear and tear and lasts as long as new.2.8-inch screen design, compact body, easy and quick to use
+18X Digital Zoom and Webcam Camera:：Easier to shoot and capture distant details,meeting the diverse needs of travel.Also it can be used as a webcam to connect to your computer via USB C cable for live streaming on YouTube/TikTok and so on
+Multi-function camera:：The vlogging camera supports multiple shooting modes to meet the daily shooting needs, simple and fast operation.And equipped with 2 batteries and a battery double charger and a 32G TF card, so that you can use without any worries
+Packing List&amp;Return Policy:：Packed with 5k digital camera,2 batteries,32G TF card,USB-C charging cable,batteries double charge,user manual and greeting card.Provide 1 year of worry-free service for the camera,respond within 12 hours.
+Good Gift for Valentine's Day, graduation season,back to school,thanksgiving, birthdays, Christmas, and other holidays or daily life(Tips:Any problem,contact us first)</t>
+  </si>
+  <si>
+    <t>imgamazon\612SAJiXXAL._AC_SL1000_.jpg</t>
+  </si>
+  <si>
+    <t>12x Optical Zoom with Optical Image Stabilizer helps you capture images with flexibility and ease
+Built-in Wi-Fi and NFC allows for easy sharing and transferring of images and videos. Large 3.0-inch LCD enables easy viewing even from a wide angle.Max Resolution:5184 x 3888
+1080p HD video capabilities, 20.2 Megapixel CMOS sensor combines with the DIGIC 4+ Image Processor to help deliver stunning image quality even in low light
+Hi-Speed USB (Mini-B), HDMI (Type D), direct connection to Canon SELPHY, PIXMA Photo Printers &amp; PictBridge compatible printers, design rule for Camera File system (DCF) compliant, DPOF (Version 1.1) compatible
+Operating temperature is 0 to 40 degree celsius. Operating humidity is 10 to 90 percent. Zooming is not possible when shooting movies Subjects look distorted when subjects that pass in front of the camera quickly may look distorted. This is not a malfunction. Shots are out of focus, press the shutter button halfway to focus on subjects before pressing it all the way down to shoot. Make sure subjects are within focusing range. Set af-assist beam to on. Confirm that unneeded functions such as macro are deactivated. Image stabilization for angular camera shake and shift-shake in macro shots hybrid-is
+Hybrid Auto lets you record up to four seconds of video before each image you capture, then automatically combines each clip and still into a quick video recap of the day
+Creative Shot mode uses composition, color and lighting from your original image to create unique images with an artistic flair
+Story Highlights enables the camera to automatically compile images and videos from a certain day or event into a mini highlight reel with music and effects.Country of origin is China</t>
+  </si>
+  <si>
+    <t>imgamazon\71mcXgTbfjL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>You’ll get well defined, detailed images thanks to the AZ401’s 16 million pixels. That’s ample resolution to crop, zoom, or enlarge your photos however the photographer in you desires.
+With a 24mm wide angle lens, there’s no sacrificing what you want in the frame. So go ahead and let your camera see what you see - the sky’s the limit!
+The Optical Image Stabilization will iron out any small movements as you’re focused on getting your shot, so you never have to be afraid to go for what you want.
+Whether you’re in the moment, or modifying your work at a later time, the bright, 3” LCD screen ensures that you end up with just what you’re looking for.
+Capture everything in your peripherals with the 180 Degree Panorama feature</t>
+  </si>
+  <si>
+    <t>imgamazon\71AK4ZCRJDL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>【12X Optical Zoom 4K UHD Video &amp; Photos】- OIEXI digital camera feature 12x optical zoom and a 13MP CMOS sensor and delivers a high bit rate of 30FPS for sharp 4K video and vibrant 64MP photos. You can also use it to photograph the moon. With anti-shake function and Built in flash, even in dim environments you can get more stable and clear images.it will be clear.allowing you to capture distant scenes without compromising on image quality, Upgraded 4K camera is a compact camera that ticks all the boxes for photographers and vloggers alike.
+【Webcam for Live Streaming &amp; HDMI Output】- This 4K digital camera can be used as a webcam, please plug in the USB cable and switch the camera to "webcam" mode, perfect for live streaming, blogging, vlogging, online teaching and more. You can also connect a TV or projector/camcorder via an HDMI cable. Not only supports an external microphone with a 3.5mm jack for clear recording, but also supports an external 1/4 standard size tripod.（Not Include） The equipped hot shoe can also connect an external fill light.（Not Include）
+【Dual Charging Options &amp; Batteries】- Our vlogging camera for youtube features dual charging options for maximum convenience. The battery charger(Not Included) allows for easy home charging, while the USB-C cable provides a portable power solution for on-the-go use. With high-capacity rechargeable batteries, you can keep shooting longer by swapping out batteries when needed. Experience uninterrupted filming and photography, and never miss a moment with this cameras for photography.meanwhile with anti-shake function and Built in flash, even in dim environments you can get more stable and clear images.
+【Multi-Functional Point &amp; Shoot Camera】- This camera for photography with a 64G SD card also has functions such as timestamp, pause, playback, compensation exposure -3.0~+3.0, slow motion, loop, continuous shooting, timed, 20+ filters.easily create the atmosphere you want! Our small and compact Vlogging camera with all the functions of a professional digital cameras. It easily fits in the jacket pocket and your purse or backpack, Also,it is really easy for you to hangs this Video camera around your neck, when and It takes great photos and it's easy to use, transferring the photos to your laptop or smart phone is quick and simple.
+【Perfect Gift for Beginners】- 4K digital camera for photography and video can be a perfect gift for Valentine's Day, graduation season, Thanksgiving, birthdays, Christmas, and other holidays or daily life. The vlogging camera can satisfy teens and adults shooting at home or traveling to record the beauty of life. For beginners, OIEXI'S cameras for photography offers the perfect starting point in photography.</t>
+  </si>
+  <si>
+    <t>imgamazon\81Wywy4nmhL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>42X Optical Zoom - 24mm Wide Angle Lens
+20 Megapixels
+1080p Full HD Video - Vlogging Camera
+SD Card Compatibility: At least Class 10, no more than 512GB (SD, SDHC, SDXC)
+3" LCD Screen - Optical Image Stabilization (OIS) - Li-Ion Battery</t>
+  </si>
+  <si>
+    <t>imgamazon\81DZOTD-aOL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>64 Mega Pixels Still Image Resolution
+4K HD Video Resolution
+16x digital zoom; 3.0 inch LCD screen
+Connect seamlessly via wifi and its smartphone app
+Uses rechargeable lithium ion battery (included); also includes 32GB memory card</t>
+  </si>
 </sst>
 </file>
 
@@ -2171,21 +3136,21 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Aptos Display"/>
+      <name val="Times New Roman"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -2193,7 +3158,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2201,7 +3166,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2209,35 +3174,35 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2245,7 +3210,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2253,14 +3218,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2268,14 +3233,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2283,7 +3248,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2291,21 +3256,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF0F1111"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3043,18 +4008,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA0270B3-C156-4102-85C1-B33FF4B3EA72}">
   <dimension ref="A1:D301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A293" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
-      <selection activeCell="A301" sqref="A301"/>
+    <sheetView tabSelected="1" topLeftCell="A179" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H182" sqref="H182"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
-    <col min="2" max="2" width="100.5546875" customWidth="1"/>
-    <col min="4" max="4" width="23.109375" customWidth="1"/>
+    <col min="1" max="1" width="43.5" customWidth="1"/>
+    <col min="2" max="2" width="100.5" customWidth="1"/>
+    <col min="4" max="4" width="23.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3068,7 +4033,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="171" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -3082,7 +4047,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -3096,7 +4061,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="199.5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3110,7 +4075,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="156.75" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -3124,7 +4089,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="171" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -3138,7 +4103,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="199.5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -3152,7 +4117,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="213.75" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -3166,7 +4131,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="216" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="213.75" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -3180,7 +4145,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="156.75" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -3194,7 +4159,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="213.75" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -3208,7 +4173,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -3222,7 +4187,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="171" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -3236,7 +4201,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -3250,7 +4215,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="288" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="299.25" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -3264,7 +4229,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="199.5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -3278,7 +4243,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -3292,7 +4257,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="199.5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -3306,7 +4271,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="171" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -3320,7 +4285,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="213.75" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -3334,7 +4299,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="242.25" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -3348,7 +4313,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="213.75" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -3362,7 +4327,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -3376,7 +4341,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -3390,7 +4355,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>52</v>
       </c>
@@ -3404,7 +4369,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="171" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>54</v>
       </c>
@@ -3418,7 +4383,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>56</v>
       </c>
@@ -3432,7 +4397,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="114" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>58</v>
       </c>
@@ -3446,7 +4411,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>60</v>
       </c>
@@ -3460,7 +4425,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="216" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="213.75" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>62</v>
       </c>
@@ -3474,7 +4439,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="156.75" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>64</v>
       </c>
@@ -3488,7 +4453,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>75</v>
       </c>
@@ -3502,7 +4467,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="114" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>77</v>
       </c>
@@ -3516,7 +4481,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>79</v>
       </c>
@@ -3530,7 +4495,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>81</v>
       </c>
@@ -3544,7 +4509,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>83</v>
       </c>
@@ -3558,7 +4523,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>85</v>
       </c>
@@ -3572,7 +4537,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>87</v>
       </c>
@@ -3586,7 +4551,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>89</v>
       </c>
@@ -3600,7 +4565,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>91</v>
       </c>
@@ -3614,7 +4579,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="242.25" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>93</v>
       </c>
@@ -3628,7 +4593,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>95</v>
       </c>
@@ -3642,7 +4607,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>97</v>
       </c>
@@ -3656,7 +4621,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="156.75" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>99</v>
       </c>
@@ -3670,7 +4635,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>101</v>
       </c>
@@ -3684,7 +4649,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>103</v>
       </c>
@@ -3698,7 +4663,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>105</v>
       </c>
@@ -3712,7 +4677,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>107</v>
       </c>
@@ -3726,7 +4691,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>109</v>
       </c>
@@ -3740,7 +4705,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>110</v>
       </c>
@@ -3754,7 +4719,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>113</v>
       </c>
@@ -3768,7 +4733,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>115</v>
       </c>
@@ -3782,7 +4747,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>107</v>
       </c>
@@ -3796,7 +4761,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>117</v>
       </c>
@@ -3810,7 +4775,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>118</v>
       </c>
@@ -3824,7 +4789,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" ht="199.5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>120</v>
       </c>
@@ -3838,7 +4803,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" ht="256.5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>122</v>
       </c>
@@ -3852,7 +4817,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" ht="199.5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>124</v>
       </c>
@@ -3866,7 +4831,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" ht="228" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>126</v>
       </c>
@@ -3880,7 +4845,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="216" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" ht="228" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>128</v>
       </c>
@@ -3894,7 +4859,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>130</v>
       </c>
@@ -3905,7 +4870,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" ht="185.25" x14ac:dyDescent="0.2">
       <c r="B62" s="1" t="s">
         <v>129</v>
       </c>
@@ -3916,7 +4881,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>132</v>
       </c>
@@ -3930,7 +4895,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" ht="228" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>134</v>
       </c>
@@ -3944,7 +4909,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" ht="228" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>136</v>
       </c>
@@ -3958,7 +4923,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>138</v>
       </c>
@@ -3972,7 +4937,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" ht="156.75" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>140</v>
       </c>
@@ -3986,7 +4951,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" ht="228" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>142</v>
       </c>
@@ -4000,7 +4965,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" ht="256.5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>140</v>
       </c>
@@ -4014,7 +4979,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" ht="114" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>145</v>
       </c>
@@ -4028,7 +4993,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" ht="142.5" x14ac:dyDescent="0.2">
       <c r="B71" s="1" t="s">
         <v>146</v>
       </c>
@@ -4039,7 +5004,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>267</v>
       </c>
@@ -4053,7 +5018,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="103.2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" ht="112.5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>269</v>
       </c>
@@ -4067,7 +5032,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" ht="285" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>271</v>
       </c>
@@ -4081,7 +5046,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" ht="156.75" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>273</v>
       </c>
@@ -4095,7 +5060,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>275</v>
       </c>
@@ -4109,7 +5074,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" ht="171" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>277</v>
       </c>
@@ -4123,7 +5088,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" ht="171" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>279</v>
       </c>
@@ -4137,7 +5102,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" ht="242.25" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>281</v>
       </c>
@@ -4151,7 +5116,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" ht="114" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>283</v>
       </c>
@@ -4165,7 +5130,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="288" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" ht="313.5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>285</v>
       </c>
@@ -4179,7 +5144,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" ht="114" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>287</v>
       </c>
@@ -4193,7 +5158,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" ht="199.5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>289</v>
       </c>
@@ -4207,7 +5172,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" ht="114" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>291</v>
       </c>
@@ -4221,7 +5186,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" ht="156.75" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>293</v>
       </c>
@@ -4235,7 +5200,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="216" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" ht="213.75" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>295</v>
       </c>
@@ -4249,7 +5214,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>297</v>
       </c>
@@ -4263,7 +5228,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" ht="171" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>299</v>
       </c>
@@ -4277,7 +5242,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>301</v>
       </c>
@@ -4291,7 +5256,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" ht="156.75" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>303</v>
       </c>
@@ -4305,7 +5270,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="288" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" ht="285" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>305</v>
       </c>
@@ -4319,7 +5284,13 @@
         <v>66</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" ht="185.25" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>426</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>427</v>
+      </c>
       <c r="C92">
         <v>4</v>
       </c>
@@ -4327,7 +5298,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>428</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>429</v>
+      </c>
       <c r="C93">
         <v>4</v>
       </c>
@@ -4335,7 +5312,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" ht="285" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>430</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>431</v>
+      </c>
       <c r="C94">
         <v>4</v>
       </c>
@@ -4343,7 +5326,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" ht="242.25" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>432</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>433</v>
+      </c>
       <c r="C95">
         <v>4</v>
       </c>
@@ -4351,7 +5340,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" ht="313.5" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>434</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>435</v>
+      </c>
       <c r="C96">
         <v>4</v>
       </c>
@@ -4359,7 +5354,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="97" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" ht="327.75" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>436</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>437</v>
+      </c>
       <c r="C97">
         <v>4</v>
       </c>
@@ -4367,7 +5368,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="98" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" ht="370.5" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>438</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>439</v>
+      </c>
       <c r="C98">
         <v>4</v>
       </c>
@@ -4375,7 +5382,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="99" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" ht="399" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>440</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>441</v>
+      </c>
       <c r="C99">
         <v>4</v>
       </c>
@@ -4383,7 +5396,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="100" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" ht="342" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>442</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>443</v>
+      </c>
       <c r="C100">
         <v>4</v>
       </c>
@@ -4391,7 +5410,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="101" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" ht="228" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>444</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>445</v>
+      </c>
       <c r="C101">
         <v>4</v>
       </c>
@@ -4399,7 +5424,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="102" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" ht="342" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>446</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>447</v>
+      </c>
       <c r="C102">
         <v>4</v>
       </c>
@@ -4407,7 +5438,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="103" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" ht="285" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>448</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>449</v>
+      </c>
       <c r="C103">
         <v>4</v>
       </c>
@@ -4415,7 +5452,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="104" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" ht="299.25" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>450</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>451</v>
+      </c>
       <c r="C104">
         <v>4</v>
       </c>
@@ -4423,7 +5466,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="105" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" ht="199.5" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>452</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>453</v>
+      </c>
       <c r="C105">
         <v>4</v>
       </c>
@@ -4431,7 +5480,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="106" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" ht="327.75" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>454</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>455</v>
+      </c>
       <c r="C106">
         <v>4</v>
       </c>
@@ -4439,7 +5494,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="107" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" ht="285" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>456</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>457</v>
+      </c>
       <c r="C107">
         <v>4</v>
       </c>
@@ -4447,7 +5508,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="108" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" ht="299.25" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>458</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>459</v>
+      </c>
       <c r="C108">
         <v>4</v>
       </c>
@@ -4455,7 +5522,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="109" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" ht="399" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>460</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>461</v>
+      </c>
       <c r="C109">
         <v>4</v>
       </c>
@@ -4463,7 +5536,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="110" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" ht="285" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>462</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>463</v>
+      </c>
       <c r="C110">
         <v>4</v>
       </c>
@@ -4471,7 +5550,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="111" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" ht="356.25" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>464</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>465</v>
+      </c>
       <c r="C111">
         <v>4</v>
       </c>
@@ -4479,7 +5564,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="112" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" ht="256.5" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>466</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>467</v>
+      </c>
       <c r="C112">
         <v>4</v>
       </c>
@@ -4487,7 +5578,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="113" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" ht="356.25" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>468</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>469</v>
+      </c>
       <c r="C113">
         <v>4</v>
       </c>
@@ -4495,7 +5592,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="114" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" ht="156.75" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>470</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>471</v>
+      </c>
       <c r="C114">
         <v>4</v>
       </c>
@@ -4503,7 +5606,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="115" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" ht="142.5" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>472</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>473</v>
+      </c>
       <c r="C115">
         <v>4</v>
       </c>
@@ -4511,7 +5620,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="116" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" ht="384.75" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>474</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>475</v>
+      </c>
       <c r="C116">
         <v>4</v>
       </c>
@@ -4519,7 +5634,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="117" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>476</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>477</v>
+      </c>
       <c r="C117">
         <v>4</v>
       </c>
@@ -4527,7 +5648,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="118" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" ht="270.75" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>478</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>479</v>
+      </c>
       <c r="C118">
         <v>4</v>
       </c>
@@ -4535,7 +5662,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="119" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>480</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>481</v>
+      </c>
       <c r="C119">
         <v>4</v>
       </c>
@@ -4543,7 +5676,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="120" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" ht="313.5" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>482</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>483</v>
+      </c>
       <c r="C120">
         <v>4</v>
       </c>
@@ -4551,7 +5690,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="121" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" ht="270.75" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>484</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>485</v>
+      </c>
       <c r="C121">
         <v>4</v>
       </c>
@@ -4559,7 +5704,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="122" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" ht="327.75" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>486</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>487</v>
+      </c>
       <c r="C122">
         <v>5</v>
       </c>
@@ -4567,7 +5718,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="123" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" ht="299.25" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>488</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>489</v>
+      </c>
       <c r="C123">
         <v>5</v>
       </c>
@@ -4575,7 +5732,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="124" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" ht="171" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>490</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>491</v>
+      </c>
       <c r="C124">
         <v>5</v>
       </c>
@@ -4583,7 +5746,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="125" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" ht="299.25" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>492</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>493</v>
+      </c>
       <c r="C125">
         <v>5</v>
       </c>
@@ -4591,7 +5760,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="126" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" ht="356.25" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>494</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>495</v>
+      </c>
       <c r="C126">
         <v>5</v>
       </c>
@@ -4599,7 +5774,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="127" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" ht="299.25" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>496</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>497</v>
+      </c>
       <c r="C127">
         <v>5</v>
       </c>
@@ -4607,7 +5788,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="128" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" ht="213.75" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>498</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>499</v>
+      </c>
       <c r="C128">
         <v>5</v>
       </c>
@@ -4615,7 +5802,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="129" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" ht="342" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>500</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>501</v>
+      </c>
       <c r="C129">
         <v>5</v>
       </c>
@@ -4623,7 +5816,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="130" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" ht="128.25" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>502</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>503</v>
+      </c>
       <c r="C130">
         <v>5</v>
       </c>
@@ -4631,7 +5830,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="131" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" ht="270.75" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>504</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>505</v>
+      </c>
       <c r="C131">
         <v>5</v>
       </c>
@@ -4639,7 +5844,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="132" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" ht="256.5" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>506</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>507</v>
+      </c>
       <c r="C132">
         <v>5</v>
       </c>
@@ -4647,7 +5858,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="133" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" ht="256.5" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>508</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>509</v>
+      </c>
       <c r="C133">
         <v>5</v>
       </c>
@@ -4655,7 +5872,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="134" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" ht="242.25" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>510</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>511</v>
+      </c>
       <c r="C134">
         <v>5</v>
       </c>
@@ -4663,7 +5886,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="135" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" ht="270.75" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>512</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>513</v>
+      </c>
       <c r="C135">
         <v>5</v>
       </c>
@@ -4671,7 +5900,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="136" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" ht="242.25" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>514</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>515</v>
+      </c>
       <c r="C136">
         <v>5</v>
       </c>
@@ -4679,7 +5914,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="137" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" ht="213.75" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>516</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>517</v>
+      </c>
       <c r="C137">
         <v>5</v>
       </c>
@@ -4687,7 +5928,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="138" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" ht="299.25" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>518</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>519</v>
+      </c>
       <c r="C138">
         <v>5</v>
       </c>
@@ -4695,7 +5942,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="139" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" ht="342" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>520</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>521</v>
+      </c>
       <c r="C139">
         <v>5</v>
       </c>
@@ -4703,7 +5956,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="140" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" ht="242.25" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>522</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>523</v>
+      </c>
       <c r="C140">
         <v>5</v>
       </c>
@@ -4711,7 +5970,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="141" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" ht="384.75" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>524</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>525</v>
+      </c>
       <c r="C141">
         <v>5</v>
       </c>
@@ -4719,7 +5984,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="142" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" ht="285" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>526</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>527</v>
+      </c>
       <c r="C142">
         <v>5</v>
       </c>
@@ -4727,7 +5998,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="143" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" ht="370.5" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>528</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>529</v>
+      </c>
       <c r="C143">
         <v>5</v>
       </c>
@@ -4735,7 +6012,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="144" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" ht="242.25" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>530</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>531</v>
+      </c>
       <c r="C144">
         <v>5</v>
       </c>
@@ -4743,7 +6026,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="145" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" ht="242.25" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>532</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>523</v>
+      </c>
       <c r="C145">
         <v>5</v>
       </c>
@@ -4751,7 +6040,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="146" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" ht="128.25" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>533</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>534</v>
+      </c>
       <c r="C146">
         <v>5</v>
       </c>
@@ -4759,7 +6054,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="147" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" ht="256.5" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>535</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>536</v>
+      </c>
       <c r="C147">
         <v>5</v>
       </c>
@@ -4767,7 +6068,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="148" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>537</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>538</v>
+      </c>
       <c r="C148">
         <v>5</v>
       </c>
@@ -4775,7 +6082,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="149" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>539</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>540</v>
+      </c>
       <c r="C149">
         <v>5</v>
       </c>
@@ -4783,7 +6096,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="150" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" ht="299.25" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>541</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>542</v>
+      </c>
       <c r="C150">
         <v>5</v>
       </c>
@@ -4791,7 +6110,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="151" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" ht="228" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>543</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>544</v>
+      </c>
       <c r="C151">
         <v>5</v>
       </c>
@@ -4799,7 +6124,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="152" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" ht="313.5" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>545</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>546</v>
+      </c>
       <c r="C152">
         <v>6</v>
       </c>
@@ -4807,7 +6138,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="153" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" ht="256.5" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>547</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>548</v>
+      </c>
       <c r="C153">
         <v>6</v>
       </c>
@@ -4815,7 +6152,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="154" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>549</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>550</v>
+      </c>
       <c r="C154">
         <v>6</v>
       </c>
@@ -4823,7 +6166,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="155" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>551</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>552</v>
+      </c>
       <c r="C155">
         <v>6</v>
       </c>
@@ -4831,7 +6180,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="156" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" ht="285" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>553</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>554</v>
+      </c>
       <c r="C156">
         <v>6</v>
       </c>
@@ -4839,7 +6194,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="157" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" ht="356.25" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>555</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>556</v>
+      </c>
       <c r="C157">
         <v>6</v>
       </c>
@@ -4847,7 +6208,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="158" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" ht="256.5" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>557</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>558</v>
+      </c>
       <c r="C158">
         <v>6</v>
       </c>
@@ -4855,7 +6222,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="159" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" ht="285" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>559</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>560</v>
+      </c>
       <c r="C159">
         <v>6</v>
       </c>
@@ -4863,7 +6236,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="160" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" ht="313.5" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>561</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>562</v>
+      </c>
       <c r="C160">
         <v>6</v>
       </c>
@@ -4871,7 +6250,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="161" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:4" ht="213.75" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>563</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>564</v>
+      </c>
       <c r="C161">
         <v>6</v>
       </c>
@@ -4879,7 +6264,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="162" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:4" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>565</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>566</v>
+      </c>
       <c r="C162">
         <v>6</v>
       </c>
@@ -4887,7 +6278,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="163" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:4" ht="299.25" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>567</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>568</v>
+      </c>
       <c r="C163">
         <v>6</v>
       </c>
@@ -4895,7 +6292,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="164" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:4" ht="313.5" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>569</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>570</v>
+      </c>
       <c r="C164">
         <v>6</v>
       </c>
@@ -4903,7 +6306,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="165" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" ht="156.75" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>571</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>572</v>
+      </c>
       <c r="C165">
         <v>6</v>
       </c>
@@ -4911,7 +6320,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="166" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:4" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>573</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>574</v>
+      </c>
       <c r="C166">
         <v>6</v>
       </c>
@@ -4919,7 +6334,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="167" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>575</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>576</v>
+      </c>
       <c r="C167">
         <v>6</v>
       </c>
@@ -4927,7 +6348,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="168" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:4" ht="270.75" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>577</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>578</v>
+      </c>
       <c r="C168">
         <v>6</v>
       </c>
@@ -4935,7 +6362,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="169" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:4" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>579</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>580</v>
+      </c>
       <c r="C169">
         <v>6</v>
       </c>
@@ -4943,7 +6376,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="170" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:4" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>581</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>582</v>
+      </c>
       <c r="C170">
         <v>6</v>
       </c>
@@ -4951,7 +6390,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="171" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:4" ht="142.5" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>583</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>584</v>
+      </c>
       <c r="C171">
         <v>6</v>
       </c>
@@ -4959,7 +6404,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="172" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:4" ht="185.25" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>585</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>586</v>
+      </c>
       <c r="C172">
         <v>6</v>
       </c>
@@ -4967,7 +6418,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="173" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:4" ht="242.25" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>587</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>588</v>
+      </c>
       <c r="C173">
         <v>6</v>
       </c>
@@ -4975,7 +6432,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="174" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:4" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>589</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>590</v>
+      </c>
       <c r="C174">
         <v>6</v>
       </c>
@@ -4983,7 +6446,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="175" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:4" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>591</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>566</v>
+      </c>
       <c r="C175">
         <v>6</v>
       </c>
@@ -4991,7 +6460,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="176" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:4" ht="242.25" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>592</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>593</v>
+      </c>
       <c r="C176">
         <v>6</v>
       </c>
@@ -4999,7 +6474,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:4" ht="270.75" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>594</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>595</v>
+      </c>
       <c r="C177">
         <v>6</v>
       </c>
@@ -5007,7 +6488,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:4" ht="128.25" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>596</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>597</v>
+      </c>
       <c r="C178">
         <v>6</v>
       </c>
@@ -5015,7 +6502,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:4" ht="370.5" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>598</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>599</v>
+      </c>
       <c r="C179">
         <v>6</v>
       </c>
@@ -5023,7 +6516,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:4" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>600</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>601</v>
+      </c>
       <c r="C180">
         <v>6</v>
       </c>
@@ -5031,7 +6530,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:4" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>602</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>603</v>
+      </c>
       <c r="C181">
         <v>6</v>
       </c>
@@ -5039,7 +6544,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="182" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:4" ht="199.5" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>245</v>
       </c>
@@ -5053,7 +6558,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:4" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>148</v>
       </c>
@@ -5067,7 +6572,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="184" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:4" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>152</v>
       </c>
@@ -5081,7 +6586,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:4" ht="156.75" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>150</v>
       </c>
@@ -5095,7 +6600,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:4" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>154</v>
       </c>
@@ -5109,7 +6614,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="216" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:4" ht="213.75" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>247</v>
       </c>
@@ -5123,7 +6628,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:4" ht="156.75" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>249</v>
       </c>
@@ -5137,7 +6642,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:4" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>251</v>
       </c>
@@ -5151,7 +6656,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:4" ht="199.5" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>159</v>
       </c>
@@ -5165,7 +6670,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="191" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:4" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>170</v>
       </c>
@@ -5179,7 +6684,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="192" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:4" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>176</v>
       </c>
@@ -5193,7 +6698,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="193" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:4" ht="199.5" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>156</v>
       </c>
@@ -5207,7 +6712,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:4" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>150</v>
       </c>
@@ -5221,7 +6726,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="195" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:4" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>158</v>
       </c>
@@ -5235,7 +6740,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="196" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:4" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>254</v>
       </c>
@@ -5249,7 +6754,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="197" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:4" ht="171" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>164</v>
       </c>
@@ -5263,7 +6768,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="198" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:4" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>166</v>
       </c>
@@ -5277,7 +6782,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="199" spans="1:4" ht="216" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:4" ht="228" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>161</v>
       </c>
@@ -5291,7 +6796,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="200" spans="1:4" ht="216" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:4" ht="228" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>172</v>
       </c>
@@ -5305,7 +6810,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="201" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:4" ht="199.5" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>180</v>
       </c>
@@ -5319,7 +6824,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="202" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:4" ht="156.75" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>255</v>
       </c>
@@ -5333,7 +6838,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="203" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:4" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>178</v>
       </c>
@@ -5347,7 +6852,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="204" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:4" ht="171" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>168</v>
       </c>
@@ -5361,7 +6866,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>257</v>
       </c>
@@ -5375,7 +6880,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="206" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>182</v>
       </c>
@@ -5389,7 +6894,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="207" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:4" ht="114" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>260</v>
       </c>
@@ -5403,7 +6908,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="208" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:4" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>174</v>
       </c>
@@ -5417,7 +6922,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="209" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:4" ht="171" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>183</v>
       </c>
@@ -5431,7 +6936,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="210" spans="1:4" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:4" ht="256.5" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>263</v>
       </c>
@@ -5445,7 +6950,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="211" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:4" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>265</v>
       </c>
@@ -5459,7 +6964,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="212" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:4" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>307</v>
       </c>
@@ -5473,7 +6978,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="213" spans="1:4" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:4" ht="242.25" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>309</v>
       </c>
@@ -5487,7 +6992,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="214" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:4" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>311</v>
       </c>
@@ -5501,7 +7006,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="215" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:4" ht="171" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>313</v>
       </c>
@@ -5515,7 +7020,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="216" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:4" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>315</v>
       </c>
@@ -5529,7 +7034,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="217" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:4" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>317</v>
       </c>
@@ -5543,7 +7048,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="218" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:4" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>319</v>
       </c>
@@ -5557,7 +7062,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="219" spans="1:4" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:4" ht="228" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>321</v>
       </c>
@@ -5571,7 +7076,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="220" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:4" ht="213.75" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>323</v>
       </c>
@@ -5585,7 +7090,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="221" spans="1:4" ht="216" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:4" ht="256.5" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>325</v>
       </c>
@@ -5599,7 +7104,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="222" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:4" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>327</v>
       </c>
@@ -5613,7 +7118,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="223" spans="1:4" ht="216" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:4" ht="213.75" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>329</v>
       </c>
@@ -5627,7 +7132,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="224" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:4" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>331</v>
       </c>
@@ -5641,7 +7146,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="225" spans="1:4" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:4" ht="256.5" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>333</v>
       </c>
@@ -5655,7 +7160,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="226" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:4" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>335</v>
       </c>
@@ -5669,7 +7174,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="227" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:4" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>337</v>
       </c>
@@ -5683,7 +7188,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="228" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:4" ht="213.75" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>339</v>
       </c>
@@ -5697,7 +7202,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="229" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:4" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>341</v>
       </c>
@@ -5711,7 +7216,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="230" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:4" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>343</v>
       </c>
@@ -5725,7 +7230,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="231" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:4" ht="114" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>345</v>
       </c>
@@ -5739,7 +7244,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="232" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:4" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>347</v>
       </c>
@@ -5753,7 +7258,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="233" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:4" ht="242.25" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>349</v>
       </c>
@@ -5767,7 +7272,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="234" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:4" ht="213.75" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>351</v>
       </c>
@@ -5781,7 +7286,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="235" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:4" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>353</v>
       </c>
@@ -5795,7 +7300,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="236" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:4" ht="199.5" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>355</v>
       </c>
@@ -5809,7 +7314,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="237" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:4" ht="156.75" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>357</v>
       </c>
@@ -5823,7 +7328,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="238" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:4" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>359</v>
       </c>
@@ -5837,7 +7342,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="239" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:4" ht="199.5" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>361</v>
       </c>
@@ -5851,7 +7356,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="240" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:4" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>363</v>
       </c>
@@ -5865,7 +7370,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="241" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:4" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>365</v>
       </c>
@@ -5879,7 +7384,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="242" spans="1:4" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:4" ht="256.5" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>185</v>
       </c>
@@ -5893,7 +7398,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="243" spans="1:4" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:4" ht="327.75" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>187</v>
       </c>
@@ -5907,7 +7412,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="244" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:4" ht="156.75" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>189</v>
       </c>
@@ -5921,7 +7426,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="245" spans="1:4" ht="216" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:4" ht="213.75" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>191</v>
       </c>
@@ -5935,7 +7440,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="246" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:4" ht="156.75" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>193</v>
       </c>
@@ -5949,7 +7454,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="247" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:4" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>195</v>
       </c>
@@ -5963,7 +7468,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="248" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:4" ht="156.75" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>196</v>
       </c>
@@ -5977,7 +7482,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="249" spans="1:4" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:4" ht="228" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>199</v>
       </c>
@@ -5991,7 +7496,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="250" spans="1:4" ht="216" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:4" ht="228" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>201</v>
       </c>
@@ -6005,7 +7510,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="251" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:4" ht="171" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>203</v>
       </c>
@@ -6019,7 +7524,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="252" spans="1:4" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:4" ht="242.25" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>205</v>
       </c>
@@ -6033,7 +7538,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="253" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:4" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>207</v>
       </c>
@@ -6047,7 +7552,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="254" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:4" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>209</v>
       </c>
@@ -6061,7 +7566,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="255" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:4" ht="199.5" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>211</v>
       </c>
@@ -6075,7 +7580,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="256" spans="1:4" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:4" ht="242.25" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>213</v>
       </c>
@@ -6089,7 +7594,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="257" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:4" ht="156.75" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>215</v>
       </c>
@@ -6103,7 +7608,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="258" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:4" ht="199.5" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>217</v>
       </c>
@@ -6117,7 +7622,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="259" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:4" ht="156.75" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>219</v>
       </c>
@@ -6131,7 +7636,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="260" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:4" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>221</v>
       </c>
@@ -6145,7 +7650,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="261" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:4" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>222</v>
       </c>
@@ -6159,7 +7664,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="262" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:4" ht="171" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>225</v>
       </c>
@@ -6173,7 +7678,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="263" spans="1:4" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:4" ht="242.25" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>227</v>
       </c>
@@ -6187,7 +7692,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="264" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:4" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>229</v>
       </c>
@@ -6201,7 +7706,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="265" spans="1:4" ht="216" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:4" ht="213.75" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>231</v>
       </c>
@@ -6215,7 +7720,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="266" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:4" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>233</v>
       </c>
@@ -6229,7 +7734,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="267" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:4" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>235</v>
       </c>
@@ -6243,7 +7748,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="268" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:4" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>237</v>
       </c>
@@ -6257,7 +7762,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="269" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:4" ht="199.5" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>239</v>
       </c>
@@ -6271,7 +7776,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="270" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:4" ht="199.5" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>241</v>
       </c>
@@ -6285,7 +7790,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="271" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:4" ht="199.5" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>243</v>
       </c>
@@ -6299,7 +7804,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="272" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:4" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>367</v>
       </c>
@@ -6313,7 +7818,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="273" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:4" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>369</v>
       </c>
@@ -6327,7 +7832,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="274" spans="1:4" ht="216" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:4" ht="213.75" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>371</v>
       </c>
@@ -6341,7 +7846,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="275" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:4" ht="171" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>373</v>
       </c>
@@ -6355,7 +7860,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="276" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:4" ht="171" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>375</v>
       </c>
@@ -6369,7 +7874,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="277" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:4" ht="156.75" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>377</v>
       </c>
@@ -6383,7 +7888,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="278" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:4" ht="171" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>379</v>
       </c>
@@ -6397,7 +7902,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="279" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:4" ht="171" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>381</v>
       </c>
@@ -6411,7 +7916,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="280" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:4" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>383</v>
       </c>
@@ -6425,7 +7930,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="281" spans="1:4" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:4" ht="256.5" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>385</v>
       </c>
@@ -6439,7 +7944,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="282" spans="1:4" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:4" ht="256.5" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>387</v>
       </c>
@@ -6453,7 +7958,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="283" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:4" ht="199.5" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>389</v>
       </c>
@@ -6467,7 +7972,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="284" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:4" ht="171" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>391</v>
       </c>
@@ -6481,7 +7986,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="285" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:4" ht="199.5" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>393</v>
       </c>
@@ -6495,7 +8000,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="286" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:4" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>395</v>
       </c>
@@ -6509,7 +8014,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="287" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:4" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>397</v>
       </c>
@@ -6523,7 +8028,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="288" spans="1:4" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:4" ht="313.5" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>399</v>
       </c>
@@ -6537,7 +8042,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="289" spans="1:4" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:4" ht="256.5" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>401</v>
       </c>
@@ -6551,7 +8056,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="290" spans="1:4" ht="216" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:4" ht="213.75" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>403</v>
       </c>
@@ -6565,7 +8070,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="291" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:4" ht="199.5" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>405</v>
       </c>
@@ -6579,7 +8084,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="292" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:4" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>407</v>
       </c>
@@ -6593,7 +8098,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="293" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:4" ht="156.75" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>409</v>
       </c>
@@ -6607,7 +8112,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="294" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:4" ht="114" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>411</v>
       </c>
@@ -6621,7 +8126,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="295" spans="1:4" ht="216" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:4" ht="270.75" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>413</v>
       </c>
@@ -6635,7 +8140,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="296" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:4" ht="156.75" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>415</v>
       </c>
@@ -6649,7 +8154,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="297" spans="1:4" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:4" ht="270.75" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>417</v>
       </c>
@@ -6663,7 +8168,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="298" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:4" ht="199.5" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>419</v>
       </c>
@@ -6677,7 +8182,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="299" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:4" ht="156.75" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>421</v>
       </c>
@@ -6691,7 +8196,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="300" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:4" ht="156.75" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>423</v>
       </c>
@@ -6705,7 +8210,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="301" spans="1:4" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:4" ht="228" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>425</v>
       </c>

</xml_diff>